<commit_message>
Fixed Regolith bugs, and updated the XLS
</commit_message>
<xml_diff>
--- a/Karbonite_RF.xlsx
+++ b/Karbonite_RF.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22340" windowHeight="13660" tabRatio="249"/>
+    <workbookView xWindow="10780" yWindow="1520" windowWidth="30400" windowHeight="18860" tabRatio="249" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Outputs" sheetId="1" r:id="rId1"/>
@@ -15,9 +15,9 @@
   <definedNames>
     <definedName name="Density">Sheet2!$A$2:$F$37</definedName>
   </definedNames>
-  <calcPr calcId="130407" iterateDelta="1E-4"/>
+  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -488,16 +488,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.000000000"/>
-    <numFmt numFmtId="165" formatCode="0.00000"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="2">
+    <numFmt numFmtId="168" formatCode="0.000000000"/>
+    <numFmt numFmtId="169" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -527,6 +523,22 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -564,8 +576,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -579,10 +603,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="168" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="13">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -599,7 +635,7 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -990,20 +1026,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:AY27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="O2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="I1" sqref="I1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:51" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="A1" s="3" t="s">
@@ -1493,7 +1532,7 @@
       </c>
       <c r="AG5" s="5" t="str">
         <f>'Config Out'!A7</f>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = UDMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH, 1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = UDMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH,  1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = UDMH, LOX_x000D_  StartActionName = Start UDMH, LOX_x000D_  StopActionName = Stop UDMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH, 1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = UDMH, LOX_x000D_  StartActionName = Start UDMH, LOX_x000D_  StopActionName = Stop UDMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH,  1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH5" s="5">
         <v>1</v>
@@ -1679,7 +1718,7 @@
       </c>
       <c r="AG7" t="str">
         <f>'Config Out'!A6</f>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NTO_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO, 1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NTO_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO,  1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NTO_x000D_  StartActionName = Start NTO_x000D_  StopActionName = Stop NTO_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO, 1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NTO_x000D_  StartActionName = Start NTO_x000D_  StopActionName = Stop NTO_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO,  1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH7">
         <v>1</v>
@@ -1895,7 +1934,7 @@
       </c>
       <c r="AG9" s="5" t="str">
         <f>'Config Out'!A20</f>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NO2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide, 550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NO2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide,  550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NO2_x000D_  StartActionName = Start NO2_x000D_  StopActionName = Stop NO2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide, 550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NO2_x000D_  StartActionName = Start NO2_x000D_  StopActionName = Stop NO2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide,  550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH9" s="5">
         <v>1</v>
@@ -1997,7 +2036,7 @@
       </c>
       <c r="AG10" t="str">
         <f>'Config Out'!A8</f>
-        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75, 1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75,  1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Ethanol75, LOX, Hzine, N2_x000D_  StartActionName = Start Ethanol75, LOX, Hzine, N2_x000D_  StopActionName = Stop Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75, 1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Ethanol75, LOX, Hzine, N2_x000D_  StartActionName = Start Ethanol75, LOX, Hzine, N2_x000D_  StopActionName = Stop Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75,  1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH10">
         <v>1</v>
@@ -2099,7 +2138,7 @@
       </c>
       <c r="AG11" t="str">
         <f>'Config Out'!A18</f>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = IRFNA-III_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III, 1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = IRFNA-III_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III,  1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = IRFNA-III_x000D_  StartActionName = Start IRFNA-III_x000D_  StopActionName = Stop IRFNA-III_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III, 1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = IRFNA-III_x000D_  StartActionName = Start IRFNA-III_x000D_  StopActionName = Stop IRFNA-III_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III,  1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH11">
         <v>1</v>
@@ -2201,7 +2240,7 @@
       </c>
       <c r="AG12" t="str">
         <f>'Config Out'!A23</f>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON15, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15, 1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON15, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15,  1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON15, N2_x000D_  StartActionName = Start MON15, N2_x000D_  StopActionName = Stop MON15, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15, 1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON15, N2_x000D_  StartActionName = Start MON15, N2_x000D_  StopActionName = Stop MON15, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15,  1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH12">
         <v>1</v>
@@ -2303,7 +2342,7 @@
       </c>
       <c r="AG13" s="5" t="str">
         <f>'Config Out'!A17</f>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine, 0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine,  0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Hzine_x000D_  StartActionName = Start Hzine_x000D_  StopActionName = Stop Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine, 0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Hzine_x000D_  StartActionName = Start Hzine_x000D_  StopActionName = Stop Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine,  0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH13" s="5">
         <v>1</v>
@@ -2411,7 +2450,7 @@
       </c>
       <c r="AG14" s="7" t="str">
         <f>'Config Out'!A21</f>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON1, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1, 1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON1, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1,  1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON1, N2_x000D_  StartActionName = Start MON1, N2_x000D_  StopActionName = Stop MON1, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1, 1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON1, N2_x000D_  StartActionName = Start MON1, N2_x000D_  StopActionName = Stop MON1, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1,  1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH14" s="7">
         <v>1</v>
@@ -2524,7 +2563,7 @@
       </c>
       <c r="AG15" s="5" t="str">
         <f>'Config Out'!A13</f>
-        <v>@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LH2, LOX, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen, 2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LH2, LOX, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen,  2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LH2, LOX, N2_x000D_  StartActionName = Start LH2, LOX, N2_x000D_  StopActionName = Stop LH2, LOX, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen, 2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LH2, LOX, N2_x000D_  StartActionName = Start LH2, LOX, N2_x000D_  StopActionName = Stop LH2, LOX, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen,  2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH15" s="5">
         <v>1</v>
@@ -2710,7 +2749,7 @@
       </c>
       <c r="AG17" t="str">
         <f>'Config Out'!A5</f>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH, 0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH,  0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MMH, LOX_x000D_  StartActionName = Start MMH, LOX_x000D_  StopActionName = Stop MMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH, 0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MMH, LOX_x000D_  StartActionName = Start MMH, LOX_x000D_  StopActionName = Stop MMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH,  0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH17">
         <v>1</v>
@@ -2890,7 +2929,7 @@
       </c>
       <c r="AG19" t="str">
         <f>'Config Out'!A22</f>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON10, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10, 1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON10, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10,  1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON10, N2_x000D_  StartActionName = Start MON10, N2_x000D_  StopActionName = Stop MON10, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10, 1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON10, N2_x000D_  StartActionName = Start MON10, N2_x000D_  StopActionName = Stop MON10, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10,  1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH19">
         <v>1</v>
@@ -2980,7 +3019,7 @@
       </c>
       <c r="AG20" t="str">
         <f>'Config Out'!A15</f>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = HTP_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP, 0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = HTP_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP,  0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = HTP_x000D_  StartActionName = Start HTP_x000D_  StopActionName = Stop HTP_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP, 0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = HTP_x000D_  StartActionName = Start HTP_x000D_  StopActionName = Stop HTP_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP,  0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="AH20">
         <v>1</v>
@@ -3479,11 +3518,10 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -3491,7 +3529,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -3501,7 +3539,7 @@
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="15.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" style="8" bestFit="1" customWidth="1"/>
@@ -4997,12 +5035,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -5010,17 +5047,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
   <dimension ref="A1:AG86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:33" s="4" customFormat="1" ht="15" customHeight="1">
       <c r="B1" s="4" t="s">
@@ -5072,37 +5112,41 @@
     <row r="2" spans="1:33" ht="15" customHeight="1">
       <c r="A2" t="str">
         <f t="shared" ref="A2:A33" si="0">B2&amp;C2&amp;D2</f>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Azine, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Aerozine50, 1.06943544155199, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Azine, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Aerozine50,  1.06943544155199, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Azine, LOX_x000D_  StartActionName = Start Azine, LOX_x000D_  StopActionName = Stop Azine, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Aerozine50, 1.06943544155199, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Azine, LOX_x000D_  StartActionName = Start Azine, LOX_x000D_  StopActionName = Stop Azine, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Aerozine50,  1.06943544155199, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B2" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E2),"",IF(Outputs!A2="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A2="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A2="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A2="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A2="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A2="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E2&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E2&amp;"
+  StartActionName = Start "&amp;$E2&amp;"
+  StopActionName = Stop "&amp;$E2&amp;"
   conversionRate = 1
   inputResources = "&amp;$G2&amp;H2&amp;L2&amp;P2&amp;"
   outputResources = "&amp;T2&amp;X2&amp;AB2&amp;AF2&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Azine, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Aerozine50, 1.06943544155199, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Azine, LOX_x000D_  StartActionName = Start Azine, LOX_x000D_  StopActionName = Stop Azine, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Aerozine50, 1.06943544155199, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="C2" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E2),"",IF(Outputs!A2="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A2="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A2="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A2="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A2="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A2="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E2&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E2&amp;"
+  StartActionName = Start "&amp;$E2&amp;"
+  StopActionName = Stop "&amp;$E2&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G2&amp;I2&amp;M2&amp;Q2&amp;"
   outputResources = "&amp;U2&amp;Y2&amp;AC2&amp;AG2&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Azine, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Aerozine50,  1.06943544155199, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Azine, LOX_x000D_  StartActionName = Start Azine, LOX_x000D_  StopActionName = Stop Azine, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Aerozine50,  1.06943544155199, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q2,Density,6,0)),Outputs!Q2,VLOOKUP(Outputs!Q2,Density,6,0))&amp;IF(ISBLANK(Outputs!U2),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U2,Density,6,0)),Outputs!U2,VLOOKUP(Outputs!U2,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y2),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y2,Density,6,0)),Outputs!Y2,VLOOKUP(Outputs!Y2,Density,6,0))&amp;IF(ISBLANK(Outputs!AC2),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC2,Density,6,0)),Outputs!AC2,VLOOKUP(Outputs!AC2,Density,6,0))))</f>
@@ -5176,37 +5220,41 @@
     <row r="3" spans="1:33" ht="15" customHeight="1">
       <c r="A3" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Hydyne, LOX, Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydyne, 1.1644502220112, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.0826714788616067, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Hydyne, LOX, Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydyne,  1.1644502220112, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.0826714788616067, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Hydyne, LOX, Hzine_x000D_  StartActionName = Start Hydyne, LOX, Hzine_x000D_  StopActionName = Stop Hydyne, LOX, Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydyne, 1.1644502220112, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.0826714788616067, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Hydyne, LOX, Hzine_x000D_  StartActionName = Start Hydyne, LOX, Hzine_x000D_  StopActionName = Stop Hydyne, LOX, Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydyne,  1.1644502220112, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.0826714788616067, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B3" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E3),"",IF(Outputs!A3="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A3="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A3="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A3="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A3="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A3="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E3&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E3&amp;"
+  StartActionName = Start "&amp;$E3&amp;"
+  StopActionName = Stop "&amp;$E3&amp;"
   conversionRate = 1
   inputResources = "&amp;$G3&amp;H3&amp;L3&amp;P3&amp;"
   outputResources = "&amp;T3&amp;X3&amp;AB3&amp;AF3&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Hydyne, LOX, Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydyne, 1.1644502220112, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.0826714788616067, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C3" t="str">
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Hydyne, LOX, Hzine_x000D_  StartActionName = Start Hydyne, LOX, Hzine_x000D_  StopActionName = Stop Hydyne, LOX, Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydyne, 1.1644502220112, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.0826714788616067, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C3" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E3),"",IF(Outputs!A3="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A3="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A3="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A3="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A3="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A3="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E3&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E3&amp;"
+  StartActionName = Start "&amp;$E3&amp;"
+  StopActionName = Stop "&amp;$E3&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G3&amp;I3&amp;M3&amp;Q3&amp;"
   outputResources = "&amp;U3&amp;Y3&amp;AC3&amp;AG3&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Hydyne, LOX, Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydyne,  1.1644502220112, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.0826714788616067, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Hydyne, LOX, Hzine_x000D_  StartActionName = Start Hydyne, LOX, Hzine_x000D_  StopActionName = Stop Hydyne, LOX, Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydyne,  1.1644502220112, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.0826714788616067, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E3" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q3,Density,6,0)),Outputs!Q3,VLOOKUP(Outputs!Q3,Density,6,0))&amp;IF(ISBLANK(Outputs!U3),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U3,Density,6,0)),Outputs!U3,VLOOKUP(Outputs!U3,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y3),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y3,Density,6,0)),Outputs!Y3,VLOOKUP(Outputs!Y3,Density,6,0))&amp;IF(ISBLANK(Outputs!AC3),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC3,Density,6,0)),Outputs!AC3,VLOOKUP(Outputs!AC3,Density,6,0))))</f>
@@ -5280,37 +5328,41 @@
     <row r="4" spans="1:33" ht="15" customHeight="1">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Ammonia, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdAmmonia, 1.02245918516123, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Ammonia, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdAmmonia,  1.02245918516123, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Ammonia, LOX_x000D_  StartActionName = Start Ammonia, LOX_x000D_  StopActionName = Stop Ammonia, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdAmmonia, 1.02245918516123, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Ammonia, LOX_x000D_  StartActionName = Start Ammonia, LOX_x000D_  StopActionName = Stop Ammonia, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdAmmonia,  1.02245918516123, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B4" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E4),"",IF(Outputs!A4="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A4="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A4="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A4="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A4="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A4="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E4&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E4&amp;"
+  StartActionName = Start "&amp;$E4&amp;"
+  StopActionName = Stop "&amp;$E4&amp;"
   conversionRate = 1
   inputResources = "&amp;$G4&amp;H4&amp;L4&amp;P4&amp;"
   outputResources = "&amp;T4&amp;X4&amp;AB4&amp;AF4&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Ammonia, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdAmmonia, 1.02245918516123, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C4" t="str">
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Ammonia, LOX_x000D_  StartActionName = Start Ammonia, LOX_x000D_  StopActionName = Stop Ammonia, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdAmmonia, 1.02245918516123, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C4" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E4),"",IF(Outputs!A4="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A4="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A4="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A4="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A4="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A4="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E4&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E4&amp;"
+  StartActionName = Start "&amp;$E4&amp;"
+  StopActionName = Stop "&amp;$E4&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G4&amp;I4&amp;M4&amp;Q4&amp;"
   outputResources = "&amp;U4&amp;Y4&amp;AC4&amp;AG4&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Ammonia, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdAmmonia,  1.02245918516123, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Ammonia, LOX_x000D_  StartActionName = Start Ammonia, LOX_x000D_  StopActionName = Stop Ammonia, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdAmmonia,  1.02245918516123, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E4" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q4,Density,6,0)),Outputs!Q4,VLOOKUP(Outputs!Q4,Density,6,0))&amp;IF(ISBLANK(Outputs!U4),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U4,Density,6,0)),Outputs!U4,VLOOKUP(Outputs!U4,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y4),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y4,Density,6,0)),Outputs!Y4,VLOOKUP(Outputs!Y4,Density,6,0))&amp;IF(ISBLANK(Outputs!AC4),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC4,Density,6,0)),Outputs!AC4,VLOOKUP(Outputs!AC4,Density,6,0))))</f>
@@ -5384,37 +5436,41 @@
     <row r="5" spans="1:33" ht="15" customHeight="1">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH, 0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH,  0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MMH, LOX_x000D_  StartActionName = Start MMH, LOX_x000D_  StopActionName = Stop MMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH, 0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MMH, LOX_x000D_  StartActionName = Start MMH, LOX_x000D_  StopActionName = Stop MMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH,  0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B5" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E5),"",IF(Outputs!A5="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A5="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A5="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A5="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A5="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A5="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E5&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E5&amp;"
+  StartActionName = Start "&amp;$E5&amp;"
+  StopActionName = Stop "&amp;$E5&amp;"
   conversionRate = 1
   inputResources = "&amp;$G5&amp;H5&amp;L5&amp;P5&amp;"
   outputResources = "&amp;T5&amp;X5&amp;AB5&amp;AF5&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH, 0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C5" t="str">
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MMH, LOX_x000D_  StartActionName = Start MMH, LOX_x000D_  StopActionName = Stop MMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH, 0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C5" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E5),"",IF(Outputs!A5="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A5="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A5="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A5="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A5="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A5="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E5&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E5&amp;"
+  StartActionName = Start "&amp;$E5&amp;"
+  StopActionName = Stop "&amp;$E5&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G5&amp;I5&amp;M5&amp;Q5&amp;"
   outputResources = "&amp;U5&amp;Y5&amp;AC5&amp;AG5&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH,  0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MMH, LOX_x000D_  StartActionName = Start MMH, LOX_x000D_  StopActionName = Stop MMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = MMH,  0.96458773988951, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E5" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q5,Density,6,0)),Outputs!Q5,VLOOKUP(Outputs!Q5,Density,6,0))&amp;IF(ISBLANK(Outputs!U5),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U5,Density,6,0)),Outputs!U5,VLOOKUP(Outputs!U5,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y5),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y5,Density,6,0)),Outputs!Y5,VLOOKUP(Outputs!Y5,Density,6,0))&amp;IF(ISBLANK(Outputs!AC5),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC5,Density,6,0)),Outputs!AC5,VLOOKUP(Outputs!AC5,Density,6,0))))</f>
@@ -5488,37 +5544,41 @@
     <row r="6" spans="1:33" ht="15" customHeight="1">
       <c r="A6" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NTO_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO, 1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NTO_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO,  1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NTO_x000D_  StartActionName = Start NTO_x000D_  StopActionName = Stop NTO_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO, 1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NTO_x000D_  StartActionName = Start NTO_x000D_  StopActionName = Stop NTO_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO,  1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B6" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E6),"",IF(Outputs!A6="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A6="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A6="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A6="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A6="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A6="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E6&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E6&amp;"
+  StartActionName = Start "&amp;$E6&amp;"
+  StopActionName = Stop "&amp;$E6&amp;"
   conversionRate = 1
   inputResources = "&amp;$G6&amp;H6&amp;L6&amp;P6&amp;"
   outputResources = "&amp;T6&amp;X6&amp;AB6&amp;AF6&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NTO_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO, 1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C6" t="str">
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NTO_x000D_  StartActionName = Start NTO_x000D_  StopActionName = Stop NTO_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO, 1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C6" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E6),"",IF(Outputs!A6="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A6="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A6="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A6="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A6="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A6="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E6&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E6&amp;"
+  StartActionName = Start "&amp;$E6&amp;"
+  StopActionName = Stop "&amp;$E6&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G6&amp;I6&amp;M6&amp;Q6&amp;"
   outputResources = "&amp;U6&amp;Y6&amp;AC6&amp;AG6&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NTO_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO,  1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NTO_x000D_  StartActionName = Start NTO_x000D_  StopActionName = Stop NTO_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = NTO,  1.15052686385799, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E6" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q6,Density,6,0)),Outputs!Q6,VLOOKUP(Outputs!Q6,Density,6,0))&amp;IF(ISBLANK(Outputs!U6),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U6,Density,6,0)),Outputs!U6,VLOOKUP(Outputs!U6,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y6),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y6,Density,6,0)),Outputs!Y6,VLOOKUP(Outputs!Y6,Density,6,0))&amp;IF(ISBLANK(Outputs!AC6),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC6,Density,6,0)),Outputs!AC6,VLOOKUP(Outputs!AC6,Density,6,0))))</f>
@@ -5592,37 +5652,41 @@
     <row r="7" spans="1:33" ht="15" customHeight="1">
       <c r="A7" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = UDMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH, 1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = UDMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH,  1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = UDMH, LOX_x000D_  StartActionName = Start UDMH, LOX_x000D_  StopActionName = Stop UDMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH, 1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = UDMH, LOX_x000D_  StartActionName = Start UDMH, LOX_x000D_  StopActionName = Stop UDMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH,  1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B7" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E7),"",IF(Outputs!A7="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A7="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A7="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A7="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A7="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A7="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E7&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E7&amp;"
+  StartActionName = Start "&amp;$E7&amp;"
+  StopActionName = Stop "&amp;$E7&amp;"
   conversionRate = 1
   inputResources = "&amp;$G7&amp;H7&amp;L7&amp;P7&amp;"
   outputResources = "&amp;T7&amp;X7&amp;AB7&amp;AF7&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = UDMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH, 1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C7" t="str">
+        <v>@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = UDMH, LOX_x000D_  StartActionName = Start UDMH, LOX_x000D_  StopActionName = Stop UDMH, LOX_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH, 1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C7" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E7),"",IF(Outputs!A7="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A7="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A7="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A7="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A7="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A7="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E7&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E7&amp;"
+  StartActionName = Start "&amp;$E7&amp;"
+  StopActionName = Stop "&amp;$E7&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G7&amp;I7&amp;M7&amp;Q7&amp;"
   outputResources = "&amp;U7&amp;Y7&amp;AC7&amp;AG7&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = UDMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH,  1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = UDMH, LOX_x000D_  StartActionName = Start UDMH, LOX_x000D_  StopActionName = Stop UDMH, LOX_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = UDMH,  1.37756107717985, False, LqdOxygen, 1.01695809636349, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E7" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q7,Density,6,0)),Outputs!Q7,VLOOKUP(Outputs!Q7,Density,6,0))&amp;IF(ISBLANK(Outputs!U7),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U7,Density,6,0)),Outputs!U7,VLOOKUP(Outputs!U7,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y7),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y7,Density,6,0)),Outputs!Y7,VLOOKUP(Outputs!Y7,Density,6,0))&amp;IF(ISBLANK(Outputs!AC7),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC7,Density,6,0)),Outputs!AC7,VLOOKUP(Outputs!AC7,Density,6,0))))</f>
@@ -5696,37 +5760,41 @@
     <row r="8" spans="1:33" ht="15" customHeight="1">
       <c r="A8" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75, 1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75,  1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Ethanol75, LOX, Hzine, N2_x000D_  StartActionName = Start Ethanol75, LOX, Hzine, N2_x000D_  StopActionName = Stop Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75, 1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Ethanol75, LOX, Hzine, N2_x000D_  StartActionName = Start Ethanol75, LOX, Hzine, N2_x000D_  StopActionName = Stop Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75,  1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B8" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E8),"",IF(Outputs!A8="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A8="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A8="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A8="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A8="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A8="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E8&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E8&amp;"
+  StartActionName = Start "&amp;$E8&amp;"
+  StopActionName = Stop "&amp;$E8&amp;"
   conversionRate = 1
   inputResources = "&amp;$G8&amp;H8&amp;L8&amp;P8&amp;"
   outputResources = "&amp;T8&amp;X8&amp;AB8&amp;AF8&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75, 1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C8" t="str">
+        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Ethanol75, LOX, Hzine, N2_x000D_  StartActionName = Start Ethanol75, LOX, Hzine, N2_x000D_  StopActionName = Stop Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75, 1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C8" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E8),"",IF(Outputs!A8="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A8="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A8="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A8="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A8="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A8="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E8&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E8&amp;"
+  StartActionName = Start "&amp;$E8&amp;"
+  StopActionName = Stop "&amp;$E8&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G8&amp;I8&amp;M8&amp;Q8&amp;"
   outputResources = "&amp;U8&amp;Y8&amp;AC8&amp;AG8&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75,  1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Ethanol75, LOX, Hzine, N2_x000D_  StartActionName = Start Ethanol75, LOX, Hzine, N2_x000D_  StopActionName = Stop Ethanol75, LOX, Hzine, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Ethanol75,  1.42631235359096, False, LqdOxygen, 0.508479048181744, True, Hydrazine, 0.289350176015623, True, Nitrogen, 203.003503054896, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E8" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q8,Density,6,0)),Outputs!Q8,VLOOKUP(Outputs!Q8,Density,6,0))&amp;IF(ISBLANK(Outputs!U8),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U8,Density,6,0)),Outputs!U8,VLOOKUP(Outputs!U8,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y8),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y8,Density,6,0)),Outputs!Y8,VLOOKUP(Outputs!Y8,Density,6,0))&amp;IF(ISBLANK(Outputs!AC8),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC8,Density,6,0)),Outputs!AC8,VLOOKUP(Outputs!AC8,Density,6,0))))</f>
@@ -5800,37 +5868,41 @@
     <row r="9" spans="1:33" ht="15" customHeight="1">
       <c r="A9" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = RP-1, LOX, Hzine, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Kerosene, 0.627716289849053, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.530475322695309, True, Nitrogen, 33.833917175816, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = RP-1, LOX, Hzine, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Kerosene,  0.627716289849053, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.530475322695309, True, Nitrogen, 33.833917175816, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = RP-1, LOX, Hzine, N2_x000D_  StartActionName = Start RP-1, LOX, Hzine, N2_x000D_  StopActionName = Stop RP-1, LOX, Hzine, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Kerosene, 0.627716289849053, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.530475322695309, True, Nitrogen, 33.833917175816, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = RP-1, LOX, Hzine, N2_x000D_  StartActionName = Start RP-1, LOX, Hzine, N2_x000D_  StopActionName = Stop RP-1, LOX, Hzine, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Kerosene,  0.627716289849053, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.530475322695309, True, Nitrogen, 33.833917175816, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B9" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E9),"",IF(Outputs!A9="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A9="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A9="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A9="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A9="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A9="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E9&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E9&amp;"
+  StartActionName = Start "&amp;$E9&amp;"
+  StopActionName = Stop "&amp;$E9&amp;"
   conversionRate = 1
   inputResources = "&amp;$G9&amp;H9&amp;L9&amp;P9&amp;"
   outputResources = "&amp;T9&amp;X9&amp;AB9&amp;AF9&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = RP-1, LOX, Hzine, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Kerosene, 0.627716289849053, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.530475322695309, True, Nitrogen, 33.833917175816, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C9" t="str">
+        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = RP-1, LOX, Hzine, N2_x000D_  StartActionName = Start RP-1, LOX, Hzine, N2_x000D_  StopActionName = Stop RP-1, LOX, Hzine, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Kerosene, 0.627716289849053, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.530475322695309, True, Nitrogen, 33.833917175816, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C9" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E9),"",IF(Outputs!A9="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A9="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A9="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A9="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A9="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A9="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E9&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E9&amp;"
+  StartActionName = Start "&amp;$E9&amp;"
+  StopActionName = Stop "&amp;$E9&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G9&amp;I9&amp;M9&amp;Q9&amp;"
   outputResources = "&amp;U9&amp;Y9&amp;AC9&amp;AG9&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = RP-1, LOX, Hzine, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Kerosene,  0.627716289849053, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.530475322695309, True, Nitrogen, 33.833917175816, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = RP-1, LOX, Hzine, N2_x000D_  StartActionName = Start RP-1, LOX, Hzine, N2_x000D_  StopActionName = Stop RP-1, LOX, Hzine, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Kerosene,  0.627716289849053, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.530475322695309, True, Nitrogen, 33.833917175816, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E9" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q9,Density,6,0)),Outputs!Q9,VLOOKUP(Outputs!Q9,Density,6,0))&amp;IF(ISBLANK(Outputs!U9),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U9,Density,6,0)),Outputs!U9,VLOOKUP(Outputs!U9,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y9),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y9,Density,6,0)),Outputs!Y9,VLOOKUP(Outputs!Y9,Density,6,0))&amp;IF(ISBLANK(Outputs!AC9),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC9,Density,6,0)),Outputs!AC9,VLOOKUP(Outputs!AC9,Density,6,0))))</f>
@@ -5904,37 +5976,41 @@
     <row r="10" spans="1:33" ht="15" customHeight="1">
       <c r="A10" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LOX, CH4, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdOxygen, 1.01695809636349, False, LqdMethane, 1.37649909470898, True, Nitrogen, 812.014012219585, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LOX, CH4, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdOxygen,  1.01695809636349, False, LqdMethane, 1.37649909470898, True, Nitrogen, 812.014012219585, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LOX, CH4, N2_x000D_  StartActionName = Start LOX, CH4, N2_x000D_  StopActionName = Stop LOX, CH4, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdOxygen, 1.01695809636349, False, LqdMethane, 1.37649909470898, True, Nitrogen, 812.014012219585, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LOX, CH4, N2_x000D_  StartActionName = Start LOX, CH4, N2_x000D_  StopActionName = Stop LOX, CH4, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdOxygen,  1.01695809636349, False, LqdMethane, 1.37649909470898, True, Nitrogen, 812.014012219585, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B10" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E10),"",IF(Outputs!A10="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A10="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A10="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A10="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A10="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A10="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E10&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E10&amp;"
+  StartActionName = Start "&amp;$E10&amp;"
+  StopActionName = Stop "&amp;$E10&amp;"
   conversionRate = 1
   inputResources = "&amp;$G10&amp;H10&amp;L10&amp;P10&amp;"
   outputResources = "&amp;T10&amp;X10&amp;AB10&amp;AF10&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LOX, CH4, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdOxygen, 1.01695809636349, False, LqdMethane, 1.37649909470898, True, Nitrogen, 812.014012219585, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C10" t="str">
+        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LOX, CH4, N2_x000D_  StartActionName = Start LOX, CH4, N2_x000D_  StopActionName = Stop LOX, CH4, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdOxygen, 1.01695809636349, False, LqdMethane, 1.37649909470898, True, Nitrogen, 812.014012219585, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C10" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E10),"",IF(Outputs!A10="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A10="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A10="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A10="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A10="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A10="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E10&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E10&amp;"
+  StartActionName = Start "&amp;$E10&amp;"
+  StopActionName = Stop "&amp;$E10&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G10&amp;I10&amp;M10&amp;Q10&amp;"
   outputResources = "&amp;U10&amp;Y10&amp;AC10&amp;AG10&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LOX, CH4, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdOxygen,  1.01695809636349, False, LqdMethane, 1.37649909470898, True, Nitrogen, 812.014012219585, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LOX, CH4, N2_x000D_  StartActionName = Start LOX, CH4, N2_x000D_  StopActionName = Stop LOX, CH4, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdOxygen,  1.01695809636349, False, LqdMethane, 1.37649909470898, True, Nitrogen, 812.014012219585, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E10" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q10,Density,6,0)),Outputs!Q10,VLOOKUP(Outputs!Q10,Density,6,0))&amp;IF(ISBLANK(Outputs!U10),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U10,Density,6,0)),Outputs!U10,VLOOKUP(Outputs!U10,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y10),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y10,Density,6,0)),Outputs!Y10,VLOOKUP(Outputs!Y10,Density,6,0))&amp;IF(ISBLANK(Outputs!AC10),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC10,Density,6,0)),Outputs!AC10,VLOOKUP(Outputs!AC10,Density,6,0))))</f>
@@ -6008,37 +6084,41 @@
     <row r="11" spans="1:33" ht="15" customHeight="1">
       <c r="A11" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = CH4, LOX, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdMethane, 1.37649909470898, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = CH4, LOX, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdMethane,  1.37649909470898, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = CH4, LOX, N2_x000D_  StartActionName = Start CH4, LOX, N2_x000D_  StopActionName = Stop CH4, LOX, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdMethane, 1.37649909470898, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = CH4, LOX, N2_x000D_  StartActionName = Start CH4, LOX, N2_x000D_  StopActionName = Stop CH4, LOX, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdMethane,  1.37649909470898, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B11" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E11),"",IF(Outputs!A11="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A11="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A11="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A11="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A11="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A11="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E11&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E11&amp;"
+  StartActionName = Start "&amp;$E11&amp;"
+  StopActionName = Stop "&amp;$E11&amp;"
   conversionRate = 1
   inputResources = "&amp;$G11&amp;H11&amp;L11&amp;P11&amp;"
   outputResources = "&amp;T11&amp;X11&amp;AB11&amp;AF11&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = CH4, LOX, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdMethane, 1.37649909470898, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C11" t="str">
+        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = CH4, LOX, N2_x000D_  StartActionName = Start CH4, LOX, N2_x000D_  StopActionName = Stop CH4, LOX, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdMethane, 1.37649909470898, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C11" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E11),"",IF(Outputs!A11="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A11="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A11="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A11="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A11="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A11="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E11&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E11&amp;"
+  StartActionName = Start "&amp;$E11&amp;"
+  StopActionName = Stop "&amp;$E11&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G11&amp;I11&amp;M11&amp;Q11&amp;"
   outputResources = "&amp;U11&amp;Y11&amp;AC11&amp;AG11&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = CH4, LOX, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdMethane,  1.37649909470898, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = CH4, LOX, N2_x000D_  StartActionName = Start CH4, LOX, N2_x000D_  StopActionName = Stop CH4, LOX, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = LqdMethane,  1.37649909470898, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E11" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q11,Density,6,0)),Outputs!Q11,VLOOKUP(Outputs!Q11,Density,6,0))&amp;IF(ISBLANK(Outputs!U11),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U11,Density,6,0)),Outputs!U11,VLOOKUP(Outputs!U11,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y11),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y11,Density,6,0)),Outputs!Y11,VLOOKUP(Outputs!Y11,Density,6,0))&amp;IF(ISBLANK(Outputs!AC11),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC11,Density,6,0)),Outputs!AC11,VLOOKUP(Outputs!AC11,Density,6,0))))</f>
@@ -6112,37 +6192,41 @@
     <row r="12" spans="1:33" ht="15" customHeight="1">
       <c r="A12" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Syntin, LOX, Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Syntin, 0.580511845887995, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.578700352031247, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Syntin, LOX, Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Syntin,  0.580511845887995, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.578700352031247, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Syntin, LOX, Hzine_x000D_  StartActionName = Start Syntin, LOX, Hzine_x000D_  StopActionName = Stop Syntin, LOX, Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Syntin, 0.580511845887995, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.578700352031247, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Syntin, LOX, Hzine_x000D_  StartActionName = Start Syntin, LOX, Hzine_x000D_  StopActionName = Stop Syntin, LOX, Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Syntin,  0.580511845887995, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.578700352031247, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B12" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E12),"",IF(Outputs!A12="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A12="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A12="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A12="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A12="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A12="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E12&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E12&amp;"
+  StartActionName = Start "&amp;$E12&amp;"
+  StopActionName = Stop "&amp;$E12&amp;"
   conversionRate = 1
   inputResources = "&amp;$G12&amp;H12&amp;L12&amp;P12&amp;"
   outputResources = "&amp;T12&amp;X12&amp;AB12&amp;AF12&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Syntin, LOX, Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Syntin, 0.580511845887995, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.578700352031247, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C12" t="str">
+        <v>@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Syntin, LOX, Hzine_x000D_  StartActionName = Start Syntin, LOX, Hzine_x000D_  StopActionName = Stop Syntin, LOX, Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Syntin, 0.580511845887995, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.578700352031247, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C12" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E12),"",IF(Outputs!A12="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A12="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A12="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A12="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A12="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A12="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E12&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E12&amp;"
+  StartActionName = Start "&amp;$E12&amp;"
+  StopActionName = Stop "&amp;$E12&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G12&amp;I12&amp;M12&amp;Q12&amp;"
   outputResources = "&amp;U12&amp;Y12&amp;AC12&amp;AG12&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Syntin, LOX, Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Syntin,  0.580511845887995, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.578700352031247, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Syntin, LOX, Hzine_x000D_  StartActionName = Start Syntin, LOX, Hzine_x000D_  StopActionName = Stop Syntin, LOX, Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Syntin,  0.580511845887995, False, LqdOxygen, 1.01695809636349, True, Hydrazine, 0.578700352031247, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E12" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q12,Density,6,0)),Outputs!Q12,VLOOKUP(Outputs!Q12,Density,6,0))&amp;IF(ISBLANK(Outputs!U12),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U12,Density,6,0)),Outputs!U12,VLOOKUP(Outputs!U12,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y12),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y12,Density,6,0)),Outputs!Y12,VLOOKUP(Outputs!Y12,Density,6,0))&amp;IF(ISBLANK(Outputs!AC12),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC12,Density,6,0)),Outputs!AC12,VLOOKUP(Outputs!AC12,Density,6,0))))</f>
@@ -6216,37 +6300,41 @@
     <row r="13" spans="1:33" ht="15" customHeight="1">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LH2, LOX, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen, 2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LH2, LOX, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen,  2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LH2, LOX, N2_x000D_  StartActionName = Start LH2, LOX, N2_x000D_  StopActionName = Stop LH2, LOX, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen, 2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LH2, LOX, N2_x000D_  StartActionName = Start LH2, LOX, N2_x000D_  StopActionName = Stop LH2, LOX, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen,  2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B13" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E13),"",IF(Outputs!A13="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A13="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A13="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A13="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A13="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A13="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E13&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E13&amp;"
+  StartActionName = Start "&amp;$E13&amp;"
+  StopActionName = Stop "&amp;$E13&amp;"
   conversionRate = 1
   inputResources = "&amp;$G13&amp;H13&amp;L13&amp;P13&amp;"
   outputResources = "&amp;T13&amp;X13&amp;AB13&amp;AF13&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LH2, LOX, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen, 2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C13" t="str">
+        <v>@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LH2, LOX, N2_x000D_  StartActionName = Start LH2, LOX, N2_x000D_  StopActionName = Stop LH2, LOX, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen, 2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C13" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E13),"",IF(Outputs!A13="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A13="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A13="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A13="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A13="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A13="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E13&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E13&amp;"
+  StartActionName = Start "&amp;$E13&amp;"
+  StopActionName = Stop "&amp;$E13&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G13&amp;I13&amp;M13&amp;Q13&amp;"
   outputResources = "&amp;U13&amp;Y13&amp;AC13&amp;AG13&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LH2, LOX, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen,  2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LH2, LOX, N2_x000D_  StartActionName = Start LH2, LOX, N2_x000D_  StopActionName = Stop LH2, LOX, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdHydrogen,  2.06352544237182, False, LqdOxygen, 1.01695809636349, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E13" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q13,Density,6,0)),Outputs!Q13,VLOOKUP(Outputs!Q13,Density,6,0))&amp;IF(ISBLANK(Outputs!U13),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U13,Density,6,0)),Outputs!U13,VLOOKUP(Outputs!U13,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y13),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y13,Density,6,0)),Outputs!Y13,VLOOKUP(Outputs!Y13,Density,6,0))&amp;IF(ISBLANK(Outputs!AC13),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC13,Density,6,0)),Outputs!AC13,VLOOKUP(Outputs!AC13,Density,6,0))))</f>
@@ -6320,37 +6408,41 @@
     <row r="14" spans="1:33" ht="15" customHeight="1">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LOX, LH2, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdOxygen, 1.01695809636349, False, LqdHydrogen, 2.06352544237182, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LOX, LH2, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdOxygen,  1.01695809636349, False, LqdHydrogen, 2.06352544237182, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LOX, LH2, N2_x000D_  StartActionName = Start LOX, LH2, N2_x000D_  StopActionName = Stop LOX, LH2, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdOxygen, 1.01695809636349, False, LqdHydrogen, 2.06352544237182, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LOX, LH2, N2_x000D_  StartActionName = Start LOX, LH2, N2_x000D_  StopActionName = Stop LOX, LH2, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdOxygen,  1.01695809636349, False, LqdHydrogen, 2.06352544237182, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B14" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E14),"",IF(Outputs!A14="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A14="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A14="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A14="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A14="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A14="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E14&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E14&amp;"
+  StartActionName = Start "&amp;$E14&amp;"
+  StopActionName = Stop "&amp;$E14&amp;"
   conversionRate = 1
   inputResources = "&amp;$G14&amp;H14&amp;L14&amp;P14&amp;"
   outputResources = "&amp;T14&amp;X14&amp;AB14&amp;AF14&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LOX, LH2, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdOxygen, 1.01695809636349, False, LqdHydrogen, 2.06352544237182, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C14" t="str">
+        <v>@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LOX, LH2, N2_x000D_  StartActionName = Start LOX, LH2, N2_x000D_  StopActionName = Stop LOX, LH2, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdOxygen, 1.01695809636349, False, LqdHydrogen, 2.06352544237182, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C14" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E14),"",IF(Outputs!A14="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A14="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A14="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A14="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A14="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A14="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E14&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E14&amp;"
+  StartActionName = Start "&amp;$E14&amp;"
+  StopActionName = Stop "&amp;$E14&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G14&amp;I14&amp;M14&amp;Q14&amp;"
   outputResources = "&amp;U14&amp;Y14&amp;AC14&amp;AG14&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = LOX, LH2, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdOxygen,  1.01695809636349, False, LqdHydrogen, 2.06352544237182, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = LOX, LH2, N2_x000D_  StartActionName = Start LOX, LH2, N2_x000D_  StopActionName = Stop LOX, LH2, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 6, Karbonite, 1_x000D_  outputResources = LqdOxygen,  1.01695809636349, False, LqdHydrogen, 2.06352544237182, True, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E14" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q14,Density,6,0)),Outputs!Q14,VLOOKUP(Outputs!Q14,Density,6,0))&amp;IF(ISBLANK(Outputs!U14),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U14,Density,6,0)),Outputs!U14,VLOOKUP(Outputs!U14,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y14),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y14,Density,6,0)),Outputs!Y14,VLOOKUP(Outputs!Y14,Density,6,0))&amp;IF(ISBLANK(Outputs!AC14),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC14,Density,6,0)),Outputs!AC14,VLOOKUP(Outputs!AC14,Density,6,0))))</f>
@@ -6424,37 +6516,41 @@
     <row r="15" spans="1:33" ht="15" customHeight="1">
       <c r="A15" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = HTP_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP, 0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = HTP_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP,  0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = HTP_x000D_  StartActionName = Start HTP_x000D_  StopActionName = Stop HTP_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP, 0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = HTP_x000D_  StartActionName = Start HTP_x000D_  StopActionName = Stop HTP_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP,  0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B15" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E15),"",IF(Outputs!A15="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A15="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A15="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A15="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A15="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A15="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E15&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E15&amp;"
+  StartActionName = Start "&amp;$E15&amp;"
+  StopActionName = Stop "&amp;$E15&amp;"
   conversionRate = 1
   inputResources = "&amp;$G15&amp;H15&amp;L15&amp;P15&amp;"
   outputResources = "&amp;T15&amp;X15&amp;AB15&amp;AF15&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = HTP_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP, 0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C15" t="str">
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = HTP_x000D_  StartActionName = Start HTP_x000D_  StopActionName = Stop HTP_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP, 0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C15" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E15),"",IF(Outputs!A15="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A15="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A15="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A15="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A15="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A15="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E15&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E15&amp;"
+  StartActionName = Start "&amp;$E15&amp;"
+  StopActionName = Stop "&amp;$E15&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G15&amp;I15&amp;M15&amp;Q15&amp;"
   outputResources = "&amp;U15&amp;Y15&amp;AC15&amp;AG15&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = HTP_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP,  0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = HTP_x000D_  StartActionName = Start HTP_x000D_  StopActionName = Stop HTP_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, LqdHydrogen, 1, LqdOxygen, 0.985651134201278_x000D_  outputResources = HTP,  0.747173715077286, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E15" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q15,Density,6,0)),Outputs!Q15,VLOOKUP(Outputs!Q15,Density,6,0))&amp;IF(ISBLANK(Outputs!U15),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U15,Density,6,0)),Outputs!U15,VLOOKUP(Outputs!U15,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y15),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y15,Density,6,0)),Outputs!Y15,VLOOKUP(Outputs!Y15,Density,6,0))&amp;IF(ISBLANK(Outputs!AC15),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC15,Density,6,0)),Outputs!AC15,VLOOKUP(Outputs!AC15,Density,6,0))))</f>
@@ -6528,37 +6624,41 @@
     <row r="16" spans="1:33" ht="15" customHeight="1">
       <c r="A16" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = HTP, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = HTP, 0.85656220607414, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = HTP, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = HTP,  0.85656220607414, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = HTP, N2_x000D_  StartActionName = Start HTP, N2_x000D_  StopActionName = Stop HTP, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = HTP, 0.85656220607414, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = HTP, N2_x000D_  StartActionName = Start HTP, N2_x000D_  StopActionName = Stop HTP, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = HTP,  0.85656220607414, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B16" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E16),"",IF(Outputs!A16="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A16="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A16="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A16="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A16="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A16="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E16&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E16&amp;"
+  StartActionName = Start "&amp;$E16&amp;"
+  StopActionName = Stop "&amp;$E16&amp;"
   conversionRate = 1
   inputResources = "&amp;$G16&amp;H16&amp;L16&amp;P16&amp;"
   outputResources = "&amp;T16&amp;X16&amp;AB16&amp;AF16&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = HTP, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = HTP, 0.85656220607414, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C16" t="str">
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = HTP, N2_x000D_  StartActionName = Start HTP, N2_x000D_  StopActionName = Stop HTP, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = HTP, 0.85656220607414, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C16" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E16),"",IF(Outputs!A16="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A16="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A16="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A16="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A16="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A16="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E16&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E16&amp;"
+  StartActionName = Start "&amp;$E16&amp;"
+  StopActionName = Stop "&amp;$E16&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G16&amp;I16&amp;M16&amp;Q16&amp;"
   outputResources = "&amp;U16&amp;Y16&amp;AC16&amp;AG16&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = HTP, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = HTP,  0.85656220607414, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = HTP, N2_x000D_  StartActionName = Start HTP, N2_x000D_  StopActionName = Stop HTP, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = HTP,  0.85656220607414, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E16" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q16,Density,6,0)),Outputs!Q16,VLOOKUP(Outputs!Q16,Density,6,0))&amp;IF(ISBLANK(Outputs!U16),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U16,Density,6,0)),Outputs!U16,VLOOKUP(Outputs!U16,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y16),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y16,Density,6,0)),Outputs!Y16,VLOOKUP(Outputs!Y16,Density,6,0))&amp;IF(ISBLANK(Outputs!AC16),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC16,Density,6,0)),Outputs!AC16,VLOOKUP(Outputs!AC16,Density,6,0))))</f>
@@ -6632,37 +6732,41 @@
     <row r="17" spans="1:33" ht="15" customHeight="1">
       <c r="A17" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine, 0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine,  0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Hzine_x000D_  StartActionName = Start Hzine_x000D_  StopActionName = Stop Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine, 0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Hzine_x000D_  StartActionName = Start Hzine_x000D_  StopActionName = Stop Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine,  0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B17" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E17),"",IF(Outputs!A17="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A17="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A17="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A17="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A17="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A17="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E17&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E17&amp;"
+  StartActionName = Start "&amp;$E17&amp;"
+  StopActionName = Stop "&amp;$E17&amp;"
   conversionRate = 1
   inputResources = "&amp;$G17&amp;H17&amp;L17&amp;P17&amp;"
   outputResources = "&amp;T17&amp;X17&amp;AB17&amp;AF17&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine, 0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C17" t="str">
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Hzine_x000D_  StartActionName = Start Hzine_x000D_  StopActionName = Stop Hzine_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine, 0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C17" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E17),"",IF(Outputs!A17="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A17="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A17="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A17="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A17="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A17="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E17&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E17&amp;"
+  StartActionName = Start "&amp;$E17&amp;"
+  StopActionName = Stop "&amp;$E17&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G17&amp;I17&amp;M17&amp;Q17&amp;"
   outputResources = "&amp;U17&amp;Y17&amp;AC17&amp;AG17&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine,  0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = Hzine_x000D_  StartActionName = Start Hzine_x000D_  StopActionName = Stop Hzine_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 2, Karbonite, 1_x000D_  outputResources = Hydrazine,  0.578700352031247, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E17" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q17,Density,6,0)),Outputs!Q17,VLOOKUP(Outputs!Q17,Density,6,0))&amp;IF(ISBLANK(Outputs!U17),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U17,Density,6,0)),Outputs!U17,VLOOKUP(Outputs!U17,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y17),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y17,Density,6,0)),Outputs!Y17,VLOOKUP(Outputs!Y17,Density,6,0))&amp;IF(ISBLANK(Outputs!AC17),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC17,Density,6,0)),Outputs!AC17,VLOOKUP(Outputs!AC17,Density,6,0))))</f>
@@ -6736,37 +6840,41 @@
     <row r="18" spans="1:33" ht="15" customHeight="1">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = IRFNA-III_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III, 1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = IRFNA-III_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III,  1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = IRFNA-III_x000D_  StartActionName = Start IRFNA-III_x000D_  StopActionName = Stop IRFNA-III_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III, 1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = IRFNA-III_x000D_  StartActionName = Start IRFNA-III_x000D_  StopActionName = Stop IRFNA-III_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III,  1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B18" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E18),"",IF(Outputs!A18="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A18="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A18="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A18="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A18="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A18="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E18&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E18&amp;"
+  StartActionName = Start "&amp;$E18&amp;"
+  StopActionName = Stop "&amp;$E18&amp;"
   conversionRate = 1
   inputResources = "&amp;$G18&amp;H18&amp;L18&amp;P18&amp;"
   outputResources = "&amp;T18&amp;X18&amp;AB18&amp;AF18&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = IRFNA-III_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III, 1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C18" t="str">
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = IRFNA-III_x000D_  StartActionName = Start IRFNA-III_x000D_  StopActionName = Stop IRFNA-III_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III, 1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C18" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E18),"",IF(Outputs!A18="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A18="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A18="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A18="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A18="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A18="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E18&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E18&amp;"
+  StartActionName = Start "&amp;$E18&amp;"
+  StopActionName = Stop "&amp;$E18&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G18&amp;I18&amp;M18&amp;Q18&amp;"
   outputResources = "&amp;U18&amp;Y18&amp;AC18&amp;AG18&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = IRFNA-III_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III,  1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = IRFNA-III_x000D_  StartActionName = Start IRFNA-III_x000D_  StopActionName = Stop IRFNA-III_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = IRFNA-III,  1.02823531181671, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E18" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q18,Density,6,0)),Outputs!Q18,VLOOKUP(Outputs!Q18,Density,6,0))&amp;IF(ISBLANK(Outputs!U18),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U18,Density,6,0)),Outputs!U18,VLOOKUP(Outputs!U18,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y18),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y18,Density,6,0)),Outputs!Y18,VLOOKUP(Outputs!Y18,Density,6,0))&amp;IF(ISBLANK(Outputs!AC18),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC18,Density,6,0)),Outputs!AC18,VLOOKUP(Outputs!AC18,Density,6,0))))</f>
@@ -6840,37 +6948,41 @@
     <row r="19" spans="1:33" ht="15" customHeight="1">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Nitrogen, 406.007006109792, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Nitrogen,  406.007006109792, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = N2_x000D_  StartActionName = Start N2_x000D_  StopActionName = Stop N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Nitrogen, 406.007006109792, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = N2_x000D_  StartActionName = Start N2_x000D_  StopActionName = Stop N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Nitrogen,  406.007006109792, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B19" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E19),"",IF(Outputs!A19="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A19="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A19="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A19="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A19="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A19="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E19&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E19&amp;"
+  StartActionName = Start "&amp;$E19&amp;"
+  StopActionName = Stop "&amp;$E19&amp;"
   conversionRate = 1
   inputResources = "&amp;$G19&amp;H19&amp;L19&amp;P19&amp;"
   outputResources = "&amp;T19&amp;X19&amp;AB19&amp;AF19&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Nitrogen, 406.007006109792, False_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C19" t="str">
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = N2_x000D_  StartActionName = Start N2_x000D_  StopActionName = Stop N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Nitrogen, 406.007006109792, False_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C19" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E19),"",IF(Outputs!A19="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A19="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A19="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A19="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A19="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A19="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E19&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E19&amp;"
+  StartActionName = Start "&amp;$E19&amp;"
+  StopActionName = Stop "&amp;$E19&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G19&amp;I19&amp;M19&amp;Q19&amp;"
   outputResources = "&amp;U19&amp;Y19&amp;AC19&amp;AG19&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Nitrogen,  406.007006109792, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = N2_x000D_  StartActionName = Start N2_x000D_  StopActionName = Stop N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = Nitrogen,  406.007006109792, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E19" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q19,Density,6,0)),Outputs!Q19,VLOOKUP(Outputs!Q19,Density,6,0))&amp;IF(ISBLANK(Outputs!U19),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U19,Density,6,0)),Outputs!U19,VLOOKUP(Outputs!U19,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y19),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y19,Density,6,0)),Outputs!Y19,VLOOKUP(Outputs!Y19,Density,6,0))&amp;IF(ISBLANK(Outputs!AC19),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC19,Density,6,0)),Outputs!AC19,VLOOKUP(Outputs!AC19,Density,6,0))))</f>
@@ -6944,37 +7056,41 @@
     <row r="20" spans="1:33" ht="15" customHeight="1">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NO2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide, 550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NO2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide,  550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NO2_x000D_  StartActionName = Start NO2_x000D_  StopActionName = Stop NO2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide, 550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NO2_x000D_  StartActionName = Start NO2_x000D_  StopActionName = Stop NO2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide,  550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B20" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E20),"",IF(Outputs!A20="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A20="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A20="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A20="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A20="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A20="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E20&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E20&amp;"
+  StartActionName = Start "&amp;$E20&amp;"
+  StopActionName = Stop "&amp;$E20&amp;"
   conversionRate = 1
   inputResources = "&amp;$G20&amp;H20&amp;L20&amp;P20&amp;"
   outputResources = "&amp;T20&amp;X20&amp;AB20&amp;AF20&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NO2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide, 550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C20" t="str">
+        <v>@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NO2_x000D_  StartActionName = Start NO2_x000D_  StopActionName = Stop NO2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide, 550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C20" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E20),"",IF(Outputs!A20="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A20="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A20="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A20="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A20="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A20="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E20&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E20&amp;"
+  StartActionName = Start "&amp;$E20&amp;"
+  StopActionName = Stop "&amp;$E20&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G20&amp;I20&amp;M20&amp;Q20&amp;"
   outputResources = "&amp;U20&amp;Y20&amp;AC20&amp;AG20&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = NO2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide,  550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = NO2_x000D_  StartActionName = Start NO2_x000D_  StopActionName = Stop NO2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.75, Karbonite, 1_x000D_  outputResources = NitrousOxide,  550.373980080283, False_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E20" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q20,Density,6,0)),Outputs!Q20,VLOOKUP(Outputs!Q20,Density,6,0))&amp;IF(ISBLANK(Outputs!U20),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U20,Density,6,0)),Outputs!U20,VLOOKUP(Outputs!U20,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y20),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y20,Density,6,0)),Outputs!Y20,VLOOKUP(Outputs!Y20,Density,6,0))&amp;IF(ISBLANK(Outputs!AC20),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC20,Density,6,0)),Outputs!AC20,VLOOKUP(Outputs!AC20,Density,6,0))))</f>
@@ -7048,37 +7164,41 @@
     <row r="21" spans="1:33" ht="15" customHeight="1">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON1, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1, 1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON1, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1,  1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON1, N2_x000D_  StartActionName = Start MON1, N2_x000D_  StopActionName = Stop MON1, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1, 1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON1, N2_x000D_  StartActionName = Start MON1, N2_x000D_  StopActionName = Stop MON1, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1,  1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B21" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E21),"",IF(Outputs!A21="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A21="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A21="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A21="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A21="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A21="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E21&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E21&amp;"
+  StartActionName = Start "&amp;$E21&amp;"
+  StopActionName = Stop "&amp;$E21&amp;"
   conversionRate = 1
   inputResources = "&amp;$G21&amp;H21&amp;L21&amp;P21&amp;"
   outputResources = "&amp;T21&amp;X21&amp;AB21&amp;AF21&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON1, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1, 1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C21" t="str">
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON1, N2_x000D_  StartActionName = Start MON1, N2_x000D_  StopActionName = Stop MON1, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1, 1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C21" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E21),"",IF(Outputs!A21="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A21="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A21="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A21="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A21="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A21="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E21&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E21&amp;"
+  StartActionName = Start "&amp;$E21&amp;"
+  StopActionName = Stop "&amp;$E21&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G21&amp;I21&amp;M21&amp;Q21&amp;"
   outputResources = "&amp;U21&amp;Y21&amp;AC21&amp;AG21&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON1, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1,  1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON1, N2_x000D_  StartActionName = Start MON1, N2_x000D_  StopActionName = Stop MON1, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON1,  1.16158537362325, False, Nitrogen, 406.007006109792, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E21" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q21,Density,6,0)),Outputs!Q21,VLOOKUP(Outputs!Q21,Density,6,0))&amp;IF(ISBLANK(Outputs!U21),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U21,Density,6,0)),Outputs!U21,VLOOKUP(Outputs!U21,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y21),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y21,Density,6,0)),Outputs!Y21,VLOOKUP(Outputs!Y21,Density,6,0))&amp;IF(ISBLANK(Outputs!AC21),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC21,Density,6,0)),Outputs!AC21,VLOOKUP(Outputs!AC21,Density,6,0))))</f>
@@ -7152,37 +7272,41 @@
     <row r="22" spans="1:33" ht="15" customHeight="1">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON10, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10, 1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON10, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10,  1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON10, N2_x000D_  StartActionName = Start MON10, N2_x000D_  StopActionName = Stop MON10, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10, 1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON10, N2_x000D_  StartActionName = Start MON10, N2_x000D_  StopActionName = Stop MON10, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10,  1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B22" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E22),"",IF(Outputs!A22="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A22="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A22="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A22="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A22="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A22="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E22&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E22&amp;"
+  StartActionName = Start "&amp;$E22&amp;"
+  StopActionName = Stop "&amp;$E22&amp;"
   conversionRate = 1
   inputResources = "&amp;$G22&amp;H22&amp;L22&amp;P22&amp;"
   outputResources = "&amp;T22&amp;X22&amp;AB22&amp;AF22&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON10, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10, 1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C22" t="str">
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON10, N2_x000D_  StartActionName = Start MON10, N2_x000D_  StopActionName = Stop MON10, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10, 1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C22" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E22),"",IF(Outputs!A22="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A22="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A22="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A22="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A22="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A22="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E22&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E22&amp;"
+  StartActionName = Start "&amp;$E22&amp;"
+  StopActionName = Stop "&amp;$E22&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G22&amp;I22&amp;M22&amp;Q22&amp;"
   outputResources = "&amp;U22&amp;Y22&amp;AC22&amp;AG22&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON10, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10,  1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON10, N2_x000D_  StartActionName = Start MON10, N2_x000D_  StopActionName = Stop MON10, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON10,  1.12639843351329, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E22" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q22,Density,6,0)),Outputs!Q22,VLOOKUP(Outputs!Q22,Density,6,0))&amp;IF(ISBLANK(Outputs!U22),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U22,Density,6,0)),Outputs!U22,VLOOKUP(Outputs!U22,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y22),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y22,Density,6,0)),Outputs!Y22,VLOOKUP(Outputs!Y22,Density,6,0))&amp;IF(ISBLANK(Outputs!AC22),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC22,Density,6,0)),Outputs!AC22,VLOOKUP(Outputs!AC22,Density,6,0))))</f>
@@ -7256,37 +7380,41 @@
     <row r="23" spans="1:33" ht="15" customHeight="1">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON15, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15, 1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON15, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15,  1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON15, N2_x000D_  StartActionName = Start MON15, N2_x000D_  StopActionName = Stop MON15, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15, 1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON15, N2_x000D_  StartActionName = Start MON15, N2_x000D_  StopActionName = Stop MON15, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15,  1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B23" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E23),"",IF(Outputs!A23="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A23="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A23="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A23="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A23="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A23="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E23&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E23&amp;"
+  StartActionName = Start "&amp;$E23&amp;"
+  StopActionName = Stop "&amp;$E23&amp;"
   conversionRate = 1
   inputResources = "&amp;$G23&amp;H23&amp;L23&amp;P23&amp;"
   outputResources = "&amp;T23&amp;X23&amp;AB23&amp;AF23&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON15, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15, 1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C23" t="str">
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON15, N2_x000D_  StartActionName = Start MON15, N2_x000D_  StopActionName = Stop MON15, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15, 1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C23" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E23),"",IF(Outputs!A23="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A23="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A23="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A23="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A23="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A23="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E23&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E23&amp;"
+  StartActionName = Start "&amp;$E23&amp;"
+  StopActionName = Stop "&amp;$E23&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G23&amp;I23&amp;M23&amp;Q23&amp;"
   outputResources = "&amp;U23&amp;Y23&amp;AC23&amp;AG23&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON15, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15,  1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON15, N2_x000D_  StartActionName = Start MON15, N2_x000D_  StopActionName = Stop MON15, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON15,  1.10461058210504, False, Nitrogen, 365.406305498813, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E23" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q23,Density,6,0)),Outputs!Q23,VLOOKUP(Outputs!Q23,Density,6,0))&amp;IF(ISBLANK(Outputs!U23),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U23,Density,6,0)),Outputs!U23,VLOOKUP(Outputs!U23,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y23),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y23,Density,6,0)),Outputs!Y23,VLOOKUP(Outputs!Y23,Density,6,0))&amp;IF(ISBLANK(Outputs!AC23),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC23,Density,6,0)),Outputs!AC23,VLOOKUP(Outputs!AC23,Density,6,0))))</f>
@@ -7360,37 +7488,41 @@
     <row r="24" spans="1:33" ht="15" customHeight="1">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON20, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON20, 1.0879995438031, False, Nitrogen, 345.105955193323, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON20, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON20,  1.0879995438031, False, Nitrogen, 345.105955193323, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON20, N2_x000D_  StartActionName = Start MON20, N2_x000D_  StopActionName = Stop MON20, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON20, 1.0879995438031, False, Nitrogen, 345.105955193323, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON20, N2_x000D_  StartActionName = Start MON20, N2_x000D_  StopActionName = Stop MON20, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON20,  1.0879995438031, False, Nitrogen, 345.105955193323, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B24" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E24),"",IF(Outputs!A24="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A24="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A24="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A24="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A24="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A24="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E24&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E24&amp;"
+  StartActionName = Start "&amp;$E24&amp;"
+  StopActionName = Stop "&amp;$E24&amp;"
   conversionRate = 1
   inputResources = "&amp;$G24&amp;H24&amp;L24&amp;P24&amp;"
   outputResources = "&amp;T24&amp;X24&amp;AB24&amp;AF24&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON20, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON20, 1.0879995438031, False, Nitrogen, 345.105955193323, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C24" t="str">
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON20, N2_x000D_  StartActionName = Start MON20, N2_x000D_  StopActionName = Stop MON20, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON20, 1.0879995438031, False, Nitrogen, 345.105955193323, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C24" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E24),"",IF(Outputs!A24="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A24="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A24="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A24="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A24="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A24="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E24&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E24&amp;"
+  StartActionName = Start "&amp;$E24&amp;"
+  StopActionName = Stop "&amp;$E24&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G24&amp;I24&amp;M24&amp;Q24&amp;"
   outputResources = "&amp;U24&amp;Y24&amp;AC24&amp;AG24&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON20, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON20,  1.0879995438031, False, Nitrogen, 345.105955193323, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON20, N2_x000D_  StartActionName = Start MON20, N2_x000D_  StopActionName = Stop MON20, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON20,  1.0879995438031, False, Nitrogen, 345.105955193323, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E24" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q24,Density,6,0)),Outputs!Q24,VLOOKUP(Outputs!Q24,Density,6,0))&amp;IF(ISBLANK(Outputs!U24),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U24,Density,6,0)),Outputs!U24,VLOOKUP(Outputs!U24,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y24),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y24,Density,6,0)),Outputs!Y24,VLOOKUP(Outputs!Y24,Density,6,0))&amp;IF(ISBLANK(Outputs!AC24),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC24,Density,6,0)),Outputs!AC24,VLOOKUP(Outputs!AC24,Density,6,0))))</f>
@@ -7464,37 +7596,41 @@
     <row r="25" spans="1:33" ht="15" customHeight="1">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON3, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON3, 1.15476096542982, False, Nitrogen, 324.805604887834, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON3, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON3,  1.15476096542982, False, Nitrogen, 324.805604887834, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON3, N2_x000D_  StartActionName = Start MON3, N2_x000D_  StopActionName = Stop MON3, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON3, 1.15476096542982, False, Nitrogen, 324.805604887834, True_x000D_ }_x000D_}_x000D__x000D_@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON3, N2_x000D_  StartActionName = Start MON3, N2_x000D_  StopActionName = Stop MON3, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON3,  1.15476096542982, False, Nitrogen, 324.805604887834, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="B25" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E25),"",IF(Outputs!A25="Distiller","@PART[KA_Distiller_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A25="DistillerM","@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A25="ConverterC","@PART[KA_Converter_250_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A25="ConverterN","@PART[KA_Converter_250_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A25="ConverterH","@PART[KA_Converter_250_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A25="ConverterO","@PART[KA_Converter_250_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E25&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E25&amp;"
+  StartActionName = Start "&amp;$E25&amp;"
+  StopActionName = Stop "&amp;$E25&amp;"
   conversionRate = 1
   inputResources = "&amp;$G25&amp;H25&amp;L25&amp;P25&amp;"
   outputResources = "&amp;T25&amp;X25&amp;AB25&amp;AF25&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON3, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON3, 1.15476096542982, False, Nitrogen, 324.805604887834, True_x000D_ }_x000D_}_x000D__x000D_</v>
-      </c>
-      <c r="C25" t="str">
+        <v>@PART[KA_Distiller_250_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON3, N2_x000D_  StartActionName = Start MON3, N2_x000D_  StopActionName = Stop MON3, N2_x000D_  conversionRate = 1_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON3, 1.15476096542982, False, Nitrogen, 324.805604887834, True_x000D_ }_x000D_}_x000D__x000D_</v>
+      </c>
+      <c r="C25" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E25),"",IF(Outputs!A25="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A25="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A25="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A25="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A25="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A25="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E25&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E25&amp;"
+  StartActionName = Start "&amp;$E25&amp;"
+  StopActionName = Stop "&amp;$E25&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G25&amp;I25&amp;M25&amp;Q25&amp;"
   outputResources = "&amp;U25&amp;Y25&amp;AC25&amp;AG25&amp;"
  }
 }
 ")</f>
-        <v>@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = USI_Converter_x000D_  converterName = MON3, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON3,  1.15476096542982, False, Nitrogen, 324.805604887834, True_x000D_ }_x000D_}_x000D__x000D_</v>
+        <v>@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]_x000D_{_x000D_ MODULE_x000D_ {_x000D_  name = REGO_ModuleResourceConverter_x000D_  ConverterName = MON3, N2_x000D_  StartActionName = Start MON3, N2_x000D_  StopActionName = Stop MON3, N2_x000D_  conversionRate = 0.5_x000D_  inputResources = ElectricCharge, 1.5, Karbonite, 1_x000D_  outputResources = MON3,  1.15476096542982, False, Nitrogen, 324.805604887834, True_x000D_ }_x000D_}_x000D__x000D_</v>
       </c>
       <c r="E25" t="str">
         <f>IF(ISBLANK(VLOOKUP(Outputs!Q25,Density,6,0)),Outputs!Q25,VLOOKUP(Outputs!Q25,Density,6,0))&amp;IF(ISBLANK(Outputs!U25),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!U25,Density,6,0)),Outputs!U25,VLOOKUP(Outputs!U25,Density,6,0)))&amp;IF(ISBLANK(Outputs!Y25),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!Y25,Density,6,0)),Outputs!Y25,VLOOKUP(Outputs!Y25,Density,6,0))&amp;IF(ISBLANK(Outputs!AC25),"",", "&amp;IF(ISBLANK(VLOOKUP(Outputs!AC25,Density,6,0)),Outputs!AC25,VLOOKUP(Outputs!AC25,Density,6,0))))</f>
@@ -7575,8 +7711,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E26&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E26&amp;"
+  StartActionName = Start "&amp;$E26&amp;"
+  StopActionName = Stop "&amp;$E26&amp;"
   conversionRate = 1
   inputResources = "&amp;$G26&amp;H26&amp;L26&amp;P26&amp;"
   outputResources = "&amp;T26&amp;X26&amp;AB26&amp;AF26&amp;"
@@ -7585,13 +7723,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C26" t="str">
+      <c r="C26" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E26),"",IF(Outputs!A26="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A26="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A26="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A26="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A26="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A26="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E26&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E26&amp;"
+  StartActionName = Start "&amp;$E26&amp;"
+  StopActionName = Stop "&amp;$E26&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G26&amp;I26&amp;M26&amp;Q26&amp;"
   outputResources = "&amp;U26&amp;Y26&amp;AC26&amp;AG26&amp;"
@@ -7679,8 +7819,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E27&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E27&amp;"
+  StartActionName = Start "&amp;$E27&amp;"
+  StopActionName = Stop "&amp;$E27&amp;"
   conversionRate = 1
   inputResources = "&amp;$G27&amp;H27&amp;L27&amp;P27&amp;"
   outputResources = "&amp;T27&amp;X27&amp;AB27&amp;AF27&amp;"
@@ -7689,13 +7831,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C27" t="str">
+      <c r="C27" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E27),"",IF(Outputs!A27="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A27="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A27="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A27="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A27="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A27="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E27&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E27&amp;"
+  StartActionName = Start "&amp;$E27&amp;"
+  StopActionName = Stop "&amp;$E27&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G27&amp;I27&amp;M27&amp;Q27&amp;"
   outputResources = "&amp;U27&amp;Y27&amp;AC27&amp;AG27&amp;"
@@ -7783,8 +7927,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E28&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E28&amp;"
+  StartActionName = Start "&amp;$E28&amp;"
+  StopActionName = Stop "&amp;$E28&amp;"
   conversionRate = 1
   inputResources = "&amp;$G28&amp;H28&amp;L28&amp;P28&amp;"
   outputResources = "&amp;T28&amp;X28&amp;AB28&amp;AF28&amp;"
@@ -7793,13 +7939,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C28" t="str">
+      <c r="C28" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E28),"",IF(Outputs!A28="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A28="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A28="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A28="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A28="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A28="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E28&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E28&amp;"
+  StartActionName = Start "&amp;$E28&amp;"
+  StopActionName = Stop "&amp;$E28&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G28&amp;I28&amp;M28&amp;Q28&amp;"
   outputResources = "&amp;U28&amp;Y28&amp;AC28&amp;AG28&amp;"
@@ -7887,8 +8035,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E29&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E29&amp;"
+  StartActionName = Start "&amp;$E29&amp;"
+  StopActionName = Stop "&amp;$E29&amp;"
   conversionRate = 1
   inputResources = "&amp;$G29&amp;H29&amp;L29&amp;P29&amp;"
   outputResources = "&amp;T29&amp;X29&amp;AB29&amp;AF29&amp;"
@@ -7897,13 +8047,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C29" t="str">
+      <c r="C29" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E29),"",IF(Outputs!A29="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A29="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A29="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A29="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A29="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A29="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E29&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E29&amp;"
+  StartActionName = Start "&amp;$E29&amp;"
+  StopActionName = Stop "&amp;$E29&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G29&amp;I29&amp;M29&amp;Q29&amp;"
   outputResources = "&amp;U29&amp;Y29&amp;AC29&amp;AG29&amp;"
@@ -7991,8 +8143,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E30&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E30&amp;"
+  StartActionName = Start "&amp;$E30&amp;"
+  StopActionName = Stop "&amp;$E30&amp;"
   conversionRate = 1
   inputResources = "&amp;$G30&amp;H30&amp;L30&amp;P30&amp;"
   outputResources = "&amp;T30&amp;X30&amp;AB30&amp;AF30&amp;"
@@ -8001,13 +8155,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C30" t="str">
+      <c r="C30" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E30),"",IF(Outputs!A30="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A30="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A30="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A30="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A30="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A30="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E30&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E30&amp;"
+  StartActionName = Start "&amp;$E30&amp;"
+  StopActionName = Stop "&amp;$E30&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G30&amp;I30&amp;M30&amp;Q30&amp;"
   outputResources = "&amp;U30&amp;Y30&amp;AC30&amp;AG30&amp;"
@@ -8095,8 +8251,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E31&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E31&amp;"
+  StartActionName = Start "&amp;$E31&amp;"
+  StopActionName = Stop "&amp;$E31&amp;"
   conversionRate = 1
   inputResources = "&amp;$G31&amp;H31&amp;L31&amp;P31&amp;"
   outputResources = "&amp;T31&amp;X31&amp;AB31&amp;AF31&amp;"
@@ -8105,13 +8263,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C31" t="str">
+      <c r="C31" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E31),"",IF(Outputs!A31="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A31="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A31="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A31="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A31="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A31="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E31&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E31&amp;"
+  StartActionName = Start "&amp;$E31&amp;"
+  StopActionName = Stop "&amp;$E31&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G31&amp;I31&amp;M31&amp;Q31&amp;"
   outputResources = "&amp;U31&amp;Y31&amp;AC31&amp;AG31&amp;"
@@ -8199,8 +8359,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E32&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E32&amp;"
+  StartActionName = Start "&amp;$E32&amp;"
+  StopActionName = Stop "&amp;$E32&amp;"
   conversionRate = 1
   inputResources = "&amp;$G32&amp;H32&amp;L32&amp;P32&amp;"
   outputResources = "&amp;T32&amp;X32&amp;AB32&amp;AF32&amp;"
@@ -8209,13 +8371,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C32" t="str">
+      <c r="C32" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E32),"",IF(Outputs!A32="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A32="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A32="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A32="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A32="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A32="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E32&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E32&amp;"
+  StartActionName = Start "&amp;$E32&amp;"
+  StopActionName = Stop "&amp;$E32&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G32&amp;I32&amp;M32&amp;Q32&amp;"
   outputResources = "&amp;U32&amp;Y32&amp;AC32&amp;AG32&amp;"
@@ -8303,8 +8467,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E33&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E33&amp;"
+  StartActionName = Start "&amp;$E33&amp;"
+  StopActionName = Stop "&amp;$E33&amp;"
   conversionRate = 1
   inputResources = "&amp;$G33&amp;H33&amp;L33&amp;P33&amp;"
   outputResources = "&amp;T33&amp;X33&amp;AB33&amp;AF33&amp;"
@@ -8313,13 +8479,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C33" t="str">
+      <c r="C33" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E33),"",IF(Outputs!A33="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A33="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A33="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A33="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A33="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A33="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E33&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E33&amp;"
+  StartActionName = Start "&amp;$E33&amp;"
+  StopActionName = Stop "&amp;$E33&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G33&amp;I33&amp;M33&amp;Q33&amp;"
   outputResources = "&amp;U33&amp;Y33&amp;AC33&amp;AG33&amp;"
@@ -8407,8 +8575,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E34&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E34&amp;"
+  StartActionName = Start "&amp;$E34&amp;"
+  StopActionName = Stop "&amp;$E34&amp;"
   conversionRate = 1
   inputResources = "&amp;$G34&amp;H34&amp;L34&amp;P34&amp;"
   outputResources = "&amp;T34&amp;X34&amp;AB34&amp;AF34&amp;"
@@ -8417,13 +8587,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C34" t="str">
+      <c r="C34" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E34),"",IF(Outputs!A34="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A34="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A34="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A34="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A34="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A34="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E34&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E34&amp;"
+  StartActionName = Start "&amp;$E34&amp;"
+  StopActionName = Stop "&amp;$E34&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G34&amp;I34&amp;M34&amp;Q34&amp;"
   outputResources = "&amp;U34&amp;Y34&amp;AC34&amp;AG34&amp;"
@@ -8511,8 +8683,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E35&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E35&amp;"
+  StartActionName = Start "&amp;$E35&amp;"
+  StopActionName = Stop "&amp;$E35&amp;"
   conversionRate = 1
   inputResources = "&amp;$G35&amp;H35&amp;L35&amp;P35&amp;"
   outputResources = "&amp;T35&amp;X35&amp;AB35&amp;AF35&amp;"
@@ -8521,13 +8695,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C35" t="str">
+      <c r="C35" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E35),"",IF(Outputs!A35="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A35="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A35="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A35="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A35="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A35="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E35&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E35&amp;"
+  StartActionName = Start "&amp;$E35&amp;"
+  StopActionName = Stop "&amp;$E35&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G35&amp;I35&amp;M35&amp;Q35&amp;"
   outputResources = "&amp;U35&amp;Y35&amp;AC35&amp;AG35&amp;"
@@ -8615,8 +8791,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E36&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E36&amp;"
+  StartActionName = Start "&amp;$E36&amp;"
+  StopActionName = Stop "&amp;$E36&amp;"
   conversionRate = 1
   inputResources = "&amp;$G36&amp;H36&amp;L36&amp;P36&amp;"
   outputResources = "&amp;T36&amp;X36&amp;AB36&amp;AF36&amp;"
@@ -8625,13 +8803,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C36" t="str">
+      <c r="C36" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E36),"",IF(Outputs!A36="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A36="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A36="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A36="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A36="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A36="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E36&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E36&amp;"
+  StartActionName = Start "&amp;$E36&amp;"
+  StopActionName = Stop "&amp;$E36&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G36&amp;I36&amp;M36&amp;Q36&amp;"
   outputResources = "&amp;U36&amp;Y36&amp;AC36&amp;AG36&amp;"
@@ -8719,8 +8899,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E37&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E37&amp;"
+  StartActionName = Start "&amp;$E37&amp;"
+  StopActionName = Stop "&amp;$E37&amp;"
   conversionRate = 1
   inputResources = "&amp;$G37&amp;H37&amp;L37&amp;P37&amp;"
   outputResources = "&amp;T37&amp;X37&amp;AB37&amp;AF37&amp;"
@@ -8729,13 +8911,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C37" t="str">
+      <c r="C37" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E37),"",IF(Outputs!A37="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A37="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A37="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A37="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A37="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A37="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E37&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E37&amp;"
+  StartActionName = Start "&amp;$E37&amp;"
+  StopActionName = Stop "&amp;$E37&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G37&amp;I37&amp;M37&amp;Q37&amp;"
   outputResources = "&amp;U37&amp;Y37&amp;AC37&amp;AG37&amp;"
@@ -8823,8 +9007,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E38&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E38&amp;"
+  StartActionName = Start "&amp;$E38&amp;"
+  StopActionName = Stop "&amp;$E38&amp;"
   conversionRate = 1
   inputResources = "&amp;$G38&amp;H38&amp;L38&amp;P38&amp;"
   outputResources = "&amp;T38&amp;X38&amp;AB38&amp;AF38&amp;"
@@ -8833,13 +9019,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C38" t="str">
+      <c r="C38" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E38),"",IF(Outputs!A38="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A38="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A38="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A38="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A38="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A38="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E38&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E38&amp;"
+  StartActionName = Start "&amp;$E38&amp;"
+  StopActionName = Stop "&amp;$E38&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G38&amp;I38&amp;M38&amp;Q38&amp;"
   outputResources = "&amp;U38&amp;Y38&amp;AC38&amp;AG38&amp;"
@@ -8927,8 +9115,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E39&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E39&amp;"
+  StartActionName = Start "&amp;$E39&amp;"
+  StopActionName = Stop "&amp;$E39&amp;"
   conversionRate = 1
   inputResources = "&amp;$G39&amp;H39&amp;L39&amp;P39&amp;"
   outputResources = "&amp;T39&amp;X39&amp;AB39&amp;AF39&amp;"
@@ -8937,13 +9127,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C39" t="str">
+      <c r="C39" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E39),"",IF(Outputs!A39="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A39="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A39="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A39="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A39="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A39="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E39&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E39&amp;"
+  StartActionName = Start "&amp;$E39&amp;"
+  StopActionName = Stop "&amp;$E39&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G39&amp;I39&amp;M39&amp;Q39&amp;"
   outputResources = "&amp;U39&amp;Y39&amp;AC39&amp;AG39&amp;"
@@ -9031,8 +9223,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E40&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E40&amp;"
+  StartActionName = Start "&amp;$E40&amp;"
+  StopActionName = Stop "&amp;$E40&amp;"
   conversionRate = 1
   inputResources = "&amp;$G40&amp;H40&amp;L40&amp;P40&amp;"
   outputResources = "&amp;T40&amp;X40&amp;AB40&amp;AF40&amp;"
@@ -9041,13 +9235,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C40" t="str">
+      <c r="C40" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E40),"",IF(Outputs!A40="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A40="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A40="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A40="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A40="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A40="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E40&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E40&amp;"
+  StartActionName = Start "&amp;$E40&amp;"
+  StopActionName = Stop "&amp;$E40&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G40&amp;I40&amp;M40&amp;Q40&amp;"
   outputResources = "&amp;U40&amp;Y40&amp;AC40&amp;AG40&amp;"
@@ -9135,8 +9331,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E41&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E41&amp;"
+  StartActionName = Start "&amp;$E41&amp;"
+  StopActionName = Stop "&amp;$E41&amp;"
   conversionRate = 1
   inputResources = "&amp;$G41&amp;H41&amp;L41&amp;P41&amp;"
   outputResources = "&amp;T41&amp;X41&amp;AB41&amp;AF41&amp;"
@@ -9145,13 +9343,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C41" t="str">
+      <c r="C41" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E41),"",IF(Outputs!A41="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A41="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A41="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A41="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A41="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A41="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E41&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E41&amp;"
+  StartActionName = Start "&amp;$E41&amp;"
+  StopActionName = Stop "&amp;$E41&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G41&amp;I41&amp;M41&amp;Q41&amp;"
   outputResources = "&amp;U41&amp;Y41&amp;AC41&amp;AG41&amp;"
@@ -9239,8 +9439,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E42&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E42&amp;"
+  StartActionName = Start "&amp;$E42&amp;"
+  StopActionName = Stop "&amp;$E42&amp;"
   conversionRate = 1
   inputResources = "&amp;$G42&amp;H42&amp;L42&amp;P42&amp;"
   outputResources = "&amp;T42&amp;X42&amp;AB42&amp;AF42&amp;"
@@ -9249,13 +9451,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C42" t="str">
+      <c r="C42" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E42),"",IF(Outputs!A42="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A42="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A42="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A42="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A42="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A42="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E42&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E42&amp;"
+  StartActionName = Start "&amp;$E42&amp;"
+  StopActionName = Stop "&amp;$E42&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G42&amp;I42&amp;M42&amp;Q42&amp;"
   outputResources = "&amp;U42&amp;Y42&amp;AC42&amp;AG42&amp;"
@@ -9343,8 +9547,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E43&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E43&amp;"
+  StartActionName = Start "&amp;$E43&amp;"
+  StopActionName = Stop "&amp;$E43&amp;"
   conversionRate = 1
   inputResources = "&amp;$G43&amp;H43&amp;L43&amp;P43&amp;"
   outputResources = "&amp;T43&amp;X43&amp;AB43&amp;AF43&amp;"
@@ -9353,13 +9559,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C43" t="str">
+      <c r="C43" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E43),"",IF(Outputs!A43="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A43="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A43="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A43="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A43="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A43="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E43&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E43&amp;"
+  StartActionName = Start "&amp;$E43&amp;"
+  StopActionName = Stop "&amp;$E43&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G43&amp;I43&amp;M43&amp;Q43&amp;"
   outputResources = "&amp;U43&amp;Y43&amp;AC43&amp;AG43&amp;"
@@ -9447,8 +9655,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E44&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E44&amp;"
+  StartActionName = Start "&amp;$E44&amp;"
+  StopActionName = Stop "&amp;$E44&amp;"
   conversionRate = 1
   inputResources = "&amp;$G44&amp;H44&amp;L44&amp;P44&amp;"
   outputResources = "&amp;T44&amp;X44&amp;AB44&amp;AF44&amp;"
@@ -9457,13 +9667,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C44" t="str">
+      <c r="C44" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E44),"",IF(Outputs!A44="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A44="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A44="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A44="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A44="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A44="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E44&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E44&amp;"
+  StartActionName = Start "&amp;$E44&amp;"
+  StopActionName = Stop "&amp;$E44&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G44&amp;I44&amp;M44&amp;Q44&amp;"
   outputResources = "&amp;U44&amp;Y44&amp;AC44&amp;AG44&amp;"
@@ -9541,7 +9753,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:33" ht="409">
       <c r="A45" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -9551,8 +9763,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E45&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E45&amp;"
+  StartActionName = Start "&amp;$E45&amp;"
+  StopActionName = Stop "&amp;$E45&amp;"
   conversionRate = 1
   inputResources = "&amp;$G45&amp;H45&amp;L45&amp;P45&amp;"
   outputResources = "&amp;T45&amp;X45&amp;AB45&amp;AF45&amp;"
@@ -9561,13 +9775,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C45" t="str">
+      <c r="C45" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E45),"",IF(Outputs!A45="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A45="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A45="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A45="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A45="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A45="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E45&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E45&amp;"
+  StartActionName = Start "&amp;$E45&amp;"
+  StopActionName = Stop "&amp;$E45&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G45&amp;I45&amp;M45&amp;Q45&amp;"
   outputResources = "&amp;U45&amp;Y45&amp;AC45&amp;AG45&amp;"
@@ -9645,7 +9861,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:33" ht="409">
       <c r="A46" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -9655,8 +9871,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E46&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E46&amp;"
+  StartActionName = Start "&amp;$E46&amp;"
+  StopActionName = Stop "&amp;$E46&amp;"
   conversionRate = 1
   inputResources = "&amp;$G46&amp;H46&amp;L46&amp;P46&amp;"
   outputResources = "&amp;T46&amp;X46&amp;AB46&amp;AF46&amp;"
@@ -9665,13 +9883,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C46" t="str">
+      <c r="C46" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E46),"",IF(Outputs!A46="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A46="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A46="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A46="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A46="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A46="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E46&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E46&amp;"
+  StartActionName = Start "&amp;$E46&amp;"
+  StopActionName = Stop "&amp;$E46&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G46&amp;I46&amp;M46&amp;Q46&amp;"
   outputResources = "&amp;U46&amp;Y46&amp;AC46&amp;AG46&amp;"
@@ -9749,7 +9969,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:33" ht="409">
       <c r="A47" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -9759,8 +9979,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E47&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E47&amp;"
+  StartActionName = Start "&amp;$E47&amp;"
+  StopActionName = Stop "&amp;$E47&amp;"
   conversionRate = 1
   inputResources = "&amp;$G47&amp;H47&amp;L47&amp;P47&amp;"
   outputResources = "&amp;T47&amp;X47&amp;AB47&amp;AF47&amp;"
@@ -9769,13 +9991,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C47" t="str">
+      <c r="C47" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E47),"",IF(Outputs!A47="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A47="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A47="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A47="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A47="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A47="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E47&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E47&amp;"
+  StartActionName = Start "&amp;$E47&amp;"
+  StopActionName = Stop "&amp;$E47&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G47&amp;I47&amp;M47&amp;Q47&amp;"
   outputResources = "&amp;U47&amp;Y47&amp;AC47&amp;AG47&amp;"
@@ -9853,7 +10077,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:33">
+    <row r="48" spans="1:33" ht="409">
       <c r="A48" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -9863,8 +10087,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E48&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E48&amp;"
+  StartActionName = Start "&amp;$E48&amp;"
+  StopActionName = Stop "&amp;$E48&amp;"
   conversionRate = 1
   inputResources = "&amp;$G48&amp;H48&amp;L48&amp;P48&amp;"
   outputResources = "&amp;T48&amp;X48&amp;AB48&amp;AF48&amp;"
@@ -9873,13 +10099,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C48" t="str">
+      <c r="C48" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E48),"",IF(Outputs!A48="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A48="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A48="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A48="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A48="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A48="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E48&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E48&amp;"
+  StartActionName = Start "&amp;$E48&amp;"
+  StopActionName = Stop "&amp;$E48&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G48&amp;I48&amp;M48&amp;Q48&amp;"
   outputResources = "&amp;U48&amp;Y48&amp;AC48&amp;AG48&amp;"
@@ -9957,7 +10185,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:33" ht="409">
       <c r="A49" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -9967,8 +10195,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E49&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E49&amp;"
+  StartActionName = Start "&amp;$E49&amp;"
+  StopActionName = Stop "&amp;$E49&amp;"
   conversionRate = 1
   inputResources = "&amp;$G49&amp;H49&amp;L49&amp;P49&amp;"
   outputResources = "&amp;T49&amp;X49&amp;AB49&amp;AF49&amp;"
@@ -9977,13 +10207,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C49" t="str">
+      <c r="C49" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E49),"",IF(Outputs!A49="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A49="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A49="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A49="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A49="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A49="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E49&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E49&amp;"
+  StartActionName = Start "&amp;$E49&amp;"
+  StopActionName = Stop "&amp;$E49&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G49&amp;I49&amp;M49&amp;Q49&amp;"
   outputResources = "&amp;U49&amp;Y49&amp;AC49&amp;AG49&amp;"
@@ -10061,7 +10293,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:33" ht="409">
       <c r="A50" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -10071,8 +10303,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E50&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E50&amp;"
+  StartActionName = Start "&amp;$E50&amp;"
+  StopActionName = Stop "&amp;$E50&amp;"
   conversionRate = 1
   inputResources = "&amp;$G50&amp;H50&amp;L50&amp;P50&amp;"
   outputResources = "&amp;T50&amp;X50&amp;AB50&amp;AF50&amp;"
@@ -10081,13 +10315,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C50" t="str">
+      <c r="C50" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E50),"",IF(Outputs!A50="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A50="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A50="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A50="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A50="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A50="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E50&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E50&amp;"
+  StartActionName = Start "&amp;$E50&amp;"
+  StopActionName = Stop "&amp;$E50&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G50&amp;I50&amp;M50&amp;Q50&amp;"
   outputResources = "&amp;U50&amp;Y50&amp;AC50&amp;AG50&amp;"
@@ -10165,7 +10401,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:33" ht="409">
       <c r="A51" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -10175,8 +10411,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E51&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E51&amp;"
+  StartActionName = Start "&amp;$E51&amp;"
+  StopActionName = Stop "&amp;$E51&amp;"
   conversionRate = 1
   inputResources = "&amp;$G51&amp;H51&amp;L51&amp;P51&amp;"
   outputResources = "&amp;T51&amp;X51&amp;AB51&amp;AF51&amp;"
@@ -10185,13 +10423,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C51" t="str">
+      <c r="C51" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E51),"",IF(Outputs!A51="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A51="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A51="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A51="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A51="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A51="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E51&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E51&amp;"
+  StartActionName = Start "&amp;$E51&amp;"
+  StopActionName = Stop "&amp;$E51&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G51&amp;I51&amp;M51&amp;Q51&amp;"
   outputResources = "&amp;U51&amp;Y51&amp;AC51&amp;AG51&amp;"
@@ -10269,7 +10509,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:33" ht="409">
       <c r="A52" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -10279,8 +10519,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E52&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E52&amp;"
+  StartActionName = Start "&amp;$E52&amp;"
+  StopActionName = Stop "&amp;$E52&amp;"
   conversionRate = 1
   inputResources = "&amp;$G52&amp;H52&amp;L52&amp;P52&amp;"
   outputResources = "&amp;T52&amp;X52&amp;AB52&amp;AF52&amp;"
@@ -10289,13 +10531,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C52" t="str">
+      <c r="C52" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E52),"",IF(Outputs!A52="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A52="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A52="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A52="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A52="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A52="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E52&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E52&amp;"
+  StartActionName = Start "&amp;$E52&amp;"
+  StopActionName = Stop "&amp;$E52&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G52&amp;I52&amp;M52&amp;Q52&amp;"
   outputResources = "&amp;U52&amp;Y52&amp;AC52&amp;AG52&amp;"
@@ -10373,7 +10617,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:33" ht="409">
       <c r="A53" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -10383,8 +10627,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E53&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E53&amp;"
+  StartActionName = Start "&amp;$E53&amp;"
+  StopActionName = Stop "&amp;$E53&amp;"
   conversionRate = 1
   inputResources = "&amp;$G53&amp;H53&amp;L53&amp;P53&amp;"
   outputResources = "&amp;T53&amp;X53&amp;AB53&amp;AF53&amp;"
@@ -10393,13 +10639,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C53" t="str">
+      <c r="C53" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E53),"",IF(Outputs!A53="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A53="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A53="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A53="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A53="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A53="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E53&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E53&amp;"
+  StartActionName = Start "&amp;$E53&amp;"
+  StopActionName = Stop "&amp;$E53&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G53&amp;I53&amp;M53&amp;Q53&amp;"
   outputResources = "&amp;U53&amp;Y53&amp;AC53&amp;AG53&amp;"
@@ -10477,7 +10725,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:33" ht="409">
       <c r="A54" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -10487,8 +10735,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E54&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E54&amp;"
+  StartActionName = Start "&amp;$E54&amp;"
+  StopActionName = Stop "&amp;$E54&amp;"
   conversionRate = 1
   inputResources = "&amp;$G54&amp;H54&amp;L54&amp;P54&amp;"
   outputResources = "&amp;T54&amp;X54&amp;AB54&amp;AF54&amp;"
@@ -10497,13 +10747,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C54" t="str">
+      <c r="C54" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E54),"",IF(Outputs!A54="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A54="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A54="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A54="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A54="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A54="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E54&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E54&amp;"
+  StartActionName = Start "&amp;$E54&amp;"
+  StopActionName = Stop "&amp;$E54&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G54&amp;I54&amp;M54&amp;Q54&amp;"
   outputResources = "&amp;U54&amp;Y54&amp;AC54&amp;AG54&amp;"
@@ -10581,7 +10833,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:33" ht="409">
       <c r="A55" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -10591,8 +10843,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E55&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E55&amp;"
+  StartActionName = Start "&amp;$E55&amp;"
+  StopActionName = Stop "&amp;$E55&amp;"
   conversionRate = 1
   inputResources = "&amp;$G55&amp;H55&amp;L55&amp;P55&amp;"
   outputResources = "&amp;T55&amp;X55&amp;AB55&amp;AF55&amp;"
@@ -10601,13 +10855,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C55" t="str">
+      <c r="C55" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E55),"",IF(Outputs!A55="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A55="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A55="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A55="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A55="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A55="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E55&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E55&amp;"
+  StartActionName = Start "&amp;$E55&amp;"
+  StopActionName = Stop "&amp;$E55&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G55&amp;I55&amp;M55&amp;Q55&amp;"
   outputResources = "&amp;U55&amp;Y55&amp;AC55&amp;AG55&amp;"
@@ -10685,7 +10941,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:33" ht="409">
       <c r="A56" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -10695,8 +10951,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E56&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E56&amp;"
+  StartActionName = Start "&amp;$E56&amp;"
+  StopActionName = Stop "&amp;$E56&amp;"
   conversionRate = 1
   inputResources = "&amp;$G56&amp;H56&amp;L56&amp;P56&amp;"
   outputResources = "&amp;T56&amp;X56&amp;AB56&amp;AF56&amp;"
@@ -10705,13 +10963,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C56" t="str">
+      <c r="C56" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E56),"",IF(Outputs!A56="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A56="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A56="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A56="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A56="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A56="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E56&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E56&amp;"
+  StartActionName = Start "&amp;$E56&amp;"
+  StopActionName = Stop "&amp;$E56&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G56&amp;I56&amp;M56&amp;Q56&amp;"
   outputResources = "&amp;U56&amp;Y56&amp;AC56&amp;AG56&amp;"
@@ -10789,7 +11049,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:33" ht="409">
       <c r="A57" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -10799,8 +11059,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E57&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E57&amp;"
+  StartActionName = Start "&amp;$E57&amp;"
+  StopActionName = Stop "&amp;$E57&amp;"
   conversionRate = 1
   inputResources = "&amp;$G57&amp;H57&amp;L57&amp;P57&amp;"
   outputResources = "&amp;T57&amp;X57&amp;AB57&amp;AF57&amp;"
@@ -10809,13 +11071,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C57" t="str">
+      <c r="C57" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E57),"",IF(Outputs!A57="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A57="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A57="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A57="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A57="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A57="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E57&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E57&amp;"
+  StartActionName = Start "&amp;$E57&amp;"
+  StopActionName = Stop "&amp;$E57&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G57&amp;I57&amp;M57&amp;Q57&amp;"
   outputResources = "&amp;U57&amp;Y57&amp;AC57&amp;AG57&amp;"
@@ -10893,7 +11157,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:33" ht="409">
       <c r="A58" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -10903,8 +11167,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E58&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E58&amp;"
+  StartActionName = Start "&amp;$E58&amp;"
+  StopActionName = Stop "&amp;$E58&amp;"
   conversionRate = 1
   inputResources = "&amp;$G58&amp;H58&amp;L58&amp;P58&amp;"
   outputResources = "&amp;T58&amp;X58&amp;AB58&amp;AF58&amp;"
@@ -10913,13 +11179,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C58" t="str">
+      <c r="C58" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E58),"",IF(Outputs!A58="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A58="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A58="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A58="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A58="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A58="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E58&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E58&amp;"
+  StartActionName = Start "&amp;$E58&amp;"
+  StopActionName = Stop "&amp;$E58&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G58&amp;I58&amp;M58&amp;Q58&amp;"
   outputResources = "&amp;U58&amp;Y58&amp;AC58&amp;AG58&amp;"
@@ -10997,7 +11265,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:33">
+    <row r="59" spans="1:33" ht="409">
       <c r="A59" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -11007,8 +11275,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E59&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E59&amp;"
+  StartActionName = Start "&amp;$E59&amp;"
+  StopActionName = Stop "&amp;$E59&amp;"
   conversionRate = 1
   inputResources = "&amp;$G59&amp;H59&amp;L59&amp;P59&amp;"
   outputResources = "&amp;T59&amp;X59&amp;AB59&amp;AF59&amp;"
@@ -11017,13 +11287,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C59" t="str">
+      <c r="C59" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E59),"",IF(Outputs!A59="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A59="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A59="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A59="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A59="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A59="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E59&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E59&amp;"
+  StartActionName = Start "&amp;$E59&amp;"
+  StopActionName = Stop "&amp;$E59&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G59&amp;I59&amp;M59&amp;Q59&amp;"
   outputResources = "&amp;U59&amp;Y59&amp;AC59&amp;AG59&amp;"
@@ -11101,7 +11373,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:33">
+    <row r="60" spans="1:33" ht="409">
       <c r="A60" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -11111,8 +11383,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E60&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E60&amp;"
+  StartActionName = Start "&amp;$E60&amp;"
+  StopActionName = Stop "&amp;$E60&amp;"
   conversionRate = 1
   inputResources = "&amp;$G60&amp;H60&amp;L60&amp;P60&amp;"
   outputResources = "&amp;T60&amp;X60&amp;AB60&amp;AF60&amp;"
@@ -11121,13 +11395,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C60" t="str">
+      <c r="C60" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E60),"",IF(Outputs!A60="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A60="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A60="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A60="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A60="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A60="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E60&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E60&amp;"
+  StartActionName = Start "&amp;$E60&amp;"
+  StopActionName = Stop "&amp;$E60&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G60&amp;I60&amp;M60&amp;Q60&amp;"
   outputResources = "&amp;U60&amp;Y60&amp;AC60&amp;AG60&amp;"
@@ -11205,7 +11481,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:33">
+    <row r="61" spans="1:33" ht="409">
       <c r="A61" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -11215,8 +11491,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E61&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E61&amp;"
+  StartActionName = Start "&amp;$E61&amp;"
+  StopActionName = Stop "&amp;$E61&amp;"
   conversionRate = 1
   inputResources = "&amp;$G61&amp;H61&amp;L61&amp;P61&amp;"
   outputResources = "&amp;T61&amp;X61&amp;AB61&amp;AF61&amp;"
@@ -11225,13 +11503,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C61" t="str">
+      <c r="C61" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E61),"",IF(Outputs!A61="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A61="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A61="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A61="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A61="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A61="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E61&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E61&amp;"
+  StartActionName = Start "&amp;$E61&amp;"
+  StopActionName = Stop "&amp;$E61&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G61&amp;I61&amp;M61&amp;Q61&amp;"
   outputResources = "&amp;U61&amp;Y61&amp;AC61&amp;AG61&amp;"
@@ -11309,7 +11589,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:33">
+    <row r="62" spans="1:33" ht="409">
       <c r="A62" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -11319,8 +11599,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E62&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E62&amp;"
+  StartActionName = Start "&amp;$E62&amp;"
+  StopActionName = Stop "&amp;$E62&amp;"
   conversionRate = 1
   inputResources = "&amp;$G62&amp;H62&amp;L62&amp;P62&amp;"
   outputResources = "&amp;T62&amp;X62&amp;AB62&amp;AF62&amp;"
@@ -11329,13 +11611,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C62" t="str">
+      <c r="C62" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E62),"",IF(Outputs!A62="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A62="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A62="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A62="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A62="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A62="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E62&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E62&amp;"
+  StartActionName = Start "&amp;$E62&amp;"
+  StopActionName = Stop "&amp;$E62&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G62&amp;I62&amp;M62&amp;Q62&amp;"
   outputResources = "&amp;U62&amp;Y62&amp;AC62&amp;AG62&amp;"
@@ -11413,7 +11697,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:33">
+    <row r="63" spans="1:33" ht="409">
       <c r="A63" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -11423,8 +11707,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E63&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E63&amp;"
+  StartActionName = Start "&amp;$E63&amp;"
+  StopActionName = Stop "&amp;$E63&amp;"
   conversionRate = 1
   inputResources = "&amp;$G63&amp;H63&amp;L63&amp;P63&amp;"
   outputResources = "&amp;T63&amp;X63&amp;AB63&amp;AF63&amp;"
@@ -11433,13 +11719,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C63" t="str">
+      <c r="C63" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E63),"",IF(Outputs!A63="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A63="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A63="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A63="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A63="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A63="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E63&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E63&amp;"
+  StartActionName = Start "&amp;$E63&amp;"
+  StopActionName = Stop "&amp;$E63&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G63&amp;I63&amp;M63&amp;Q63&amp;"
   outputResources = "&amp;U63&amp;Y63&amp;AC63&amp;AG63&amp;"
@@ -11517,7 +11805,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:33">
+    <row r="64" spans="1:33" ht="409">
       <c r="A64" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -11527,8 +11815,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E64&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E64&amp;"
+  StartActionName = Start "&amp;$E64&amp;"
+  StopActionName = Stop "&amp;$E64&amp;"
   conversionRate = 1
   inputResources = "&amp;$G64&amp;H64&amp;L64&amp;P64&amp;"
   outputResources = "&amp;T64&amp;X64&amp;AB64&amp;AF64&amp;"
@@ -11537,13 +11827,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C64" t="str">
+      <c r="C64" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E64),"",IF(Outputs!A64="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A64="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A64="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A64="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A64="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A64="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E64&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E64&amp;"
+  StartActionName = Start "&amp;$E64&amp;"
+  StopActionName = Stop "&amp;$E64&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G64&amp;I64&amp;M64&amp;Q64&amp;"
   outputResources = "&amp;U64&amp;Y64&amp;AC64&amp;AG64&amp;"
@@ -11621,7 +11913,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:33">
+    <row r="65" spans="1:33" ht="409">
       <c r="A65" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -11631,8 +11923,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E65&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E65&amp;"
+  StartActionName = Start "&amp;$E65&amp;"
+  StopActionName = Stop "&amp;$E65&amp;"
   conversionRate = 1
   inputResources = "&amp;$G65&amp;H65&amp;L65&amp;P65&amp;"
   outputResources = "&amp;T65&amp;X65&amp;AB65&amp;AF65&amp;"
@@ -11641,13 +11935,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C65" t="str">
+      <c r="C65" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E65),"",IF(Outputs!A65="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A65="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A65="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A65="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A65="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A65="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E65&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E65&amp;"
+  StartActionName = Start "&amp;$E65&amp;"
+  StopActionName = Stop "&amp;$E65&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G65&amp;I65&amp;M65&amp;Q65&amp;"
   outputResources = "&amp;U65&amp;Y65&amp;AC65&amp;AG65&amp;"
@@ -11725,9 +12021,9 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:33">
+    <row r="66" spans="1:33" ht="409">
       <c r="A66" t="str">
-        <f t="shared" ref="A66:A97" si="2">B66&amp;C66&amp;D66</f>
+        <f t="shared" ref="A66:A86" si="2">B66&amp;C66&amp;D66</f>
         <v/>
       </c>
       <c r="B66" s="6" t="str">
@@ -11735,8 +12031,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E66&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E66&amp;"
+  StartActionName = Start "&amp;$E66&amp;"
+  StopActionName = Stop "&amp;$E66&amp;"
   conversionRate = 1
   inputResources = "&amp;$G66&amp;H66&amp;L66&amp;P66&amp;"
   outputResources = "&amp;T66&amp;X66&amp;AB66&amp;AF66&amp;"
@@ -11745,13 +12043,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C66" t="str">
+      <c r="C66" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E66),"",IF(Outputs!A66="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A66="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A66="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A66="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A66="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A66="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E66&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E66&amp;"
+  StartActionName = Start "&amp;$E66&amp;"
+  StopActionName = Stop "&amp;$E66&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G66&amp;I66&amp;M66&amp;Q66&amp;"
   outputResources = "&amp;U66&amp;Y66&amp;AC66&amp;AG66&amp;"
@@ -11829,7 +12129,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:33">
+    <row r="67" spans="1:33" ht="409">
       <c r="A67" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -11839,8 +12139,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E67&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E67&amp;"
+  StartActionName = Start "&amp;$E67&amp;"
+  StopActionName = Stop "&amp;$E67&amp;"
   conversionRate = 1
   inputResources = "&amp;$G67&amp;H67&amp;L67&amp;P67&amp;"
   outputResources = "&amp;T67&amp;X67&amp;AB67&amp;AF67&amp;"
@@ -11849,13 +12151,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C67" t="str">
+      <c r="C67" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E67),"",IF(Outputs!A67="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A67="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A67="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A67="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A67="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A67="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E67&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E67&amp;"
+  StartActionName = Start "&amp;$E67&amp;"
+  StopActionName = Stop "&amp;$E67&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G67&amp;I67&amp;M67&amp;Q67&amp;"
   outputResources = "&amp;U67&amp;Y67&amp;AC67&amp;AG67&amp;"
@@ -11933,7 +12237,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:33">
+    <row r="68" spans="1:33" ht="409">
       <c r="A68" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -11943,8 +12247,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E68&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E68&amp;"
+  StartActionName = Start "&amp;$E68&amp;"
+  StopActionName = Stop "&amp;$E68&amp;"
   conversionRate = 1
   inputResources = "&amp;$G68&amp;H68&amp;L68&amp;P68&amp;"
   outputResources = "&amp;T68&amp;X68&amp;AB68&amp;AF68&amp;"
@@ -11953,13 +12259,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C68" t="str">
+      <c r="C68" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E68),"",IF(Outputs!A68="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A68="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A68="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A68="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A68="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A68="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E68&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E68&amp;"
+  StartActionName = Start "&amp;$E68&amp;"
+  StopActionName = Stop "&amp;$E68&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G68&amp;I68&amp;M68&amp;Q68&amp;"
   outputResources = "&amp;U68&amp;Y68&amp;AC68&amp;AG68&amp;"
@@ -12037,7 +12345,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:33">
+    <row r="69" spans="1:33" ht="409">
       <c r="A69" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12047,8 +12355,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E69&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E69&amp;"
+  StartActionName = Start "&amp;$E69&amp;"
+  StopActionName = Stop "&amp;$E69&amp;"
   conversionRate = 1
   inputResources = "&amp;$G69&amp;H69&amp;L69&amp;P69&amp;"
   outputResources = "&amp;T69&amp;X69&amp;AB69&amp;AF69&amp;"
@@ -12057,13 +12367,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C69" t="str">
+      <c r="C69" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E69),"",IF(Outputs!A69="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A69="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A69="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A69="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A69="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A69="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E69&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E69&amp;"
+  StartActionName = Start "&amp;$E69&amp;"
+  StopActionName = Stop "&amp;$E69&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G69&amp;I69&amp;M69&amp;Q69&amp;"
   outputResources = "&amp;U69&amp;Y69&amp;AC69&amp;AG69&amp;"
@@ -12141,7 +12453,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:33">
+    <row r="70" spans="1:33" ht="409">
       <c r="A70" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12151,8 +12463,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E70&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E70&amp;"
+  StartActionName = Start "&amp;$E70&amp;"
+  StopActionName = Stop "&amp;$E70&amp;"
   conversionRate = 1
   inputResources = "&amp;$G70&amp;H70&amp;L70&amp;P70&amp;"
   outputResources = "&amp;T70&amp;X70&amp;AB70&amp;AF70&amp;"
@@ -12161,13 +12475,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C70" t="str">
+      <c r="C70" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E70),"",IF(Outputs!A70="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A70="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A70="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A70="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A70="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A70="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E70&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E70&amp;"
+  StartActionName = Start "&amp;$E70&amp;"
+  StopActionName = Stop "&amp;$E70&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G70&amp;I70&amp;M70&amp;Q70&amp;"
   outputResources = "&amp;U70&amp;Y70&amp;AC70&amp;AG70&amp;"
@@ -12245,7 +12561,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:33">
+    <row r="71" spans="1:33" ht="409">
       <c r="A71" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12255,8 +12571,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E71&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E71&amp;"
+  StartActionName = Start "&amp;$E71&amp;"
+  StopActionName = Stop "&amp;$E71&amp;"
   conversionRate = 1
   inputResources = "&amp;$G71&amp;H71&amp;L71&amp;P71&amp;"
   outputResources = "&amp;T71&amp;X71&amp;AB71&amp;AF71&amp;"
@@ -12265,13 +12583,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C71" t="str">
+      <c r="C71" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E71),"",IF(Outputs!A71="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A71="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A71="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A71="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A71="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A71="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E71&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E71&amp;"
+  StartActionName = Start "&amp;$E71&amp;"
+  StopActionName = Stop "&amp;$E71&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G71&amp;I71&amp;M71&amp;Q71&amp;"
   outputResources = "&amp;U71&amp;Y71&amp;AC71&amp;AG71&amp;"
@@ -12349,7 +12669,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:33">
+    <row r="72" spans="1:33" ht="409">
       <c r="A72" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12359,8 +12679,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E72&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E72&amp;"
+  StartActionName = Start "&amp;$E72&amp;"
+  StopActionName = Stop "&amp;$E72&amp;"
   conversionRate = 1
   inputResources = "&amp;$G72&amp;H72&amp;L72&amp;P72&amp;"
   outputResources = "&amp;T72&amp;X72&amp;AB72&amp;AF72&amp;"
@@ -12369,13 +12691,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C72" t="str">
+      <c r="C72" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E72),"",IF(Outputs!A72="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A72="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A72="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A72="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A72="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A72="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E72&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E72&amp;"
+  StartActionName = Start "&amp;$E72&amp;"
+  StopActionName = Stop "&amp;$E72&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G72&amp;I72&amp;M72&amp;Q72&amp;"
   outputResources = "&amp;U72&amp;Y72&amp;AC72&amp;AG72&amp;"
@@ -12453,7 +12777,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:33">
+    <row r="73" spans="1:33" ht="409">
       <c r="A73" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12463,8 +12787,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E73&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E73&amp;"
+  StartActionName = Start "&amp;$E73&amp;"
+  StopActionName = Stop "&amp;$E73&amp;"
   conversionRate = 1
   inputResources = "&amp;$G73&amp;H73&amp;L73&amp;P73&amp;"
   outputResources = "&amp;T73&amp;X73&amp;AB73&amp;AF73&amp;"
@@ -12473,13 +12799,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C73" t="str">
+      <c r="C73" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E73),"",IF(Outputs!A73="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A73="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A73="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A73="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A73="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A73="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E73&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E73&amp;"
+  StartActionName = Start "&amp;$E73&amp;"
+  StopActionName = Stop "&amp;$E73&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G73&amp;I73&amp;M73&amp;Q73&amp;"
   outputResources = "&amp;U73&amp;Y73&amp;AC73&amp;AG73&amp;"
@@ -12557,7 +12885,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:33">
+    <row r="74" spans="1:33" ht="409">
       <c r="A74" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12567,8 +12895,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E74&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E74&amp;"
+  StartActionName = Start "&amp;$E74&amp;"
+  StopActionName = Stop "&amp;$E74&amp;"
   conversionRate = 1
   inputResources = "&amp;$G74&amp;H74&amp;L74&amp;P74&amp;"
   outputResources = "&amp;T74&amp;X74&amp;AB74&amp;AF74&amp;"
@@ -12577,13 +12907,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C74" t="str">
+      <c r="C74" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E74),"",IF(Outputs!A74="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A74="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A74="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A74="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A74="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A74="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E74&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E74&amp;"
+  StartActionName = Start "&amp;$E74&amp;"
+  StopActionName = Stop "&amp;$E74&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G74&amp;I74&amp;M74&amp;Q74&amp;"
   outputResources = "&amp;U74&amp;Y74&amp;AC74&amp;AG74&amp;"
@@ -12661,7 +12993,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:33">
+    <row r="75" spans="1:33" ht="409">
       <c r="A75" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12671,8 +13003,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E75&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E75&amp;"
+  StartActionName = Start "&amp;$E75&amp;"
+  StopActionName = Stop "&amp;$E75&amp;"
   conversionRate = 1
   inputResources = "&amp;$G75&amp;H75&amp;L75&amp;P75&amp;"
   outputResources = "&amp;T75&amp;X75&amp;AB75&amp;AF75&amp;"
@@ -12681,13 +13015,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C75" t="str">
+      <c r="C75" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E75),"",IF(Outputs!A75="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A75="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A75="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A75="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A75="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A75="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E75&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E75&amp;"
+  StartActionName = Start "&amp;$E75&amp;"
+  StopActionName = Stop "&amp;$E75&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G75&amp;I75&amp;M75&amp;Q75&amp;"
   outputResources = "&amp;U75&amp;Y75&amp;AC75&amp;AG75&amp;"
@@ -12765,7 +13101,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:33">
+    <row r="76" spans="1:33" ht="409">
       <c r="A76" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12775,8 +13111,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E76&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E76&amp;"
+  StartActionName = Start "&amp;$E76&amp;"
+  StopActionName = Stop "&amp;$E76&amp;"
   conversionRate = 1
   inputResources = "&amp;$G76&amp;H76&amp;L76&amp;P76&amp;"
   outputResources = "&amp;T76&amp;X76&amp;AB76&amp;AF76&amp;"
@@ -12785,13 +13123,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C76" t="str">
+      <c r="C76" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E76),"",IF(Outputs!A76="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A76="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A76="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A76="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A76="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A76="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E76&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E76&amp;"
+  StartActionName = Start "&amp;$E76&amp;"
+  StopActionName = Stop "&amp;$E76&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G76&amp;I76&amp;M76&amp;Q76&amp;"
   outputResources = "&amp;U76&amp;Y76&amp;AC76&amp;AG76&amp;"
@@ -12869,7 +13209,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:33">
+    <row r="77" spans="1:33" ht="409">
       <c r="A77" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12879,8 +13219,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E77&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E77&amp;"
+  StartActionName = Start "&amp;$E77&amp;"
+  StopActionName = Stop "&amp;$E77&amp;"
   conversionRate = 1
   inputResources = "&amp;$G77&amp;H77&amp;L77&amp;P77&amp;"
   outputResources = "&amp;T77&amp;X77&amp;AB77&amp;AF77&amp;"
@@ -12889,13 +13231,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C77" t="str">
+      <c r="C77" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E77),"",IF(Outputs!A77="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A77="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A77="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A77="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A77="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A77="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E77&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E77&amp;"
+  StartActionName = Start "&amp;$E77&amp;"
+  StopActionName = Stop "&amp;$E77&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G77&amp;I77&amp;M77&amp;Q77&amp;"
   outputResources = "&amp;U77&amp;Y77&amp;AC77&amp;AG77&amp;"
@@ -12973,7 +13317,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:33">
+    <row r="78" spans="1:33" ht="409">
       <c r="A78" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -12983,8 +13327,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E78&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E78&amp;"
+  StartActionName = Start "&amp;$E78&amp;"
+  StopActionName = Stop "&amp;$E78&amp;"
   conversionRate = 1
   inputResources = "&amp;$G78&amp;H78&amp;L78&amp;P78&amp;"
   outputResources = "&amp;T78&amp;X78&amp;AB78&amp;AF78&amp;"
@@ -12993,13 +13339,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C78" t="str">
+      <c r="C78" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E78),"",IF(Outputs!A78="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A78="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A78="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A78="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A78="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A78="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E78&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E78&amp;"
+  StartActionName = Start "&amp;$E78&amp;"
+  StopActionName = Stop "&amp;$E78&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G78&amp;I78&amp;M78&amp;Q78&amp;"
   outputResources = "&amp;U78&amp;Y78&amp;AC78&amp;AG78&amp;"
@@ -13077,7 +13425,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:33">
+    <row r="79" spans="1:33" ht="409">
       <c r="A79" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -13087,8 +13435,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E79&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E79&amp;"
+  StartActionName = Start "&amp;$E79&amp;"
+  StopActionName = Stop "&amp;$E79&amp;"
   conversionRate = 1
   inputResources = "&amp;$G79&amp;H79&amp;L79&amp;P79&amp;"
   outputResources = "&amp;T79&amp;X79&amp;AB79&amp;AF79&amp;"
@@ -13097,13 +13447,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C79" t="str">
+      <c r="C79" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E79),"",IF(Outputs!A79="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A79="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A79="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A79="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A79="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A79="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E79&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E79&amp;"
+  StartActionName = Start "&amp;$E79&amp;"
+  StopActionName = Stop "&amp;$E79&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G79&amp;I79&amp;M79&amp;Q79&amp;"
   outputResources = "&amp;U79&amp;Y79&amp;AC79&amp;AG79&amp;"
@@ -13181,7 +13533,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:33">
+    <row r="80" spans="1:33" ht="409">
       <c r="A80" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -13191,8 +13543,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E80&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E80&amp;"
+  StartActionName = Start "&amp;$E80&amp;"
+  StopActionName = Stop "&amp;$E80&amp;"
   conversionRate = 1
   inputResources = "&amp;$G80&amp;H80&amp;L80&amp;P80&amp;"
   outputResources = "&amp;T80&amp;X80&amp;AB80&amp;AF80&amp;"
@@ -13201,13 +13555,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C80" t="str">
+      <c r="C80" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E80),"",IF(Outputs!A80="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A80="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A80="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A80="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A80="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A80="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E80&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E80&amp;"
+  StartActionName = Start "&amp;$E80&amp;"
+  StopActionName = Stop "&amp;$E80&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G80&amp;I80&amp;M80&amp;Q80&amp;"
   outputResources = "&amp;U80&amp;Y80&amp;AC80&amp;AG80&amp;"
@@ -13285,7 +13641,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:33">
+    <row r="81" spans="1:33" ht="409">
       <c r="A81" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -13295,8 +13651,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E81&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E81&amp;"
+  StartActionName = Start "&amp;$E81&amp;"
+  StopActionName = Stop "&amp;$E81&amp;"
   conversionRate = 1
   inputResources = "&amp;$G81&amp;H81&amp;L81&amp;P81&amp;"
   outputResources = "&amp;T81&amp;X81&amp;AB81&amp;AF81&amp;"
@@ -13305,13 +13663,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C81" t="str">
+      <c r="C81" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E81),"",IF(Outputs!A81="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A81="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A81="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A81="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A81="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A81="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E81&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E81&amp;"
+  StartActionName = Start "&amp;$E81&amp;"
+  StopActionName = Stop "&amp;$E81&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G81&amp;I81&amp;M81&amp;Q81&amp;"
   outputResources = "&amp;U81&amp;Y81&amp;AC81&amp;AG81&amp;"
@@ -13389,7 +13749,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:33">
+    <row r="82" spans="1:33" ht="409">
       <c r="A82" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -13399,8 +13759,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E82&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E82&amp;"
+  StartActionName = Start "&amp;$E82&amp;"
+  StopActionName = Stop "&amp;$E82&amp;"
   conversionRate = 1
   inputResources = "&amp;$G82&amp;H82&amp;L82&amp;P82&amp;"
   outputResources = "&amp;T82&amp;X82&amp;AB82&amp;AF82&amp;"
@@ -13409,13 +13771,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C82" t="str">
+      <c r="C82" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E82),"",IF(Outputs!A82="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A82="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A82="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A82="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A82="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A82="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E82&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E82&amp;"
+  StartActionName = Start "&amp;$E82&amp;"
+  StopActionName = Stop "&amp;$E82&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G82&amp;I82&amp;M82&amp;Q82&amp;"
   outputResources = "&amp;U82&amp;Y82&amp;AC82&amp;AG82&amp;"
@@ -13493,7 +13857,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:33">
+    <row r="83" spans="1:33" ht="409">
       <c r="A83" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -13503,8 +13867,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E83&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E83&amp;"
+  StartActionName = Start "&amp;$E83&amp;"
+  StopActionName = Stop "&amp;$E83&amp;"
   conversionRate = 1
   inputResources = "&amp;$G83&amp;H83&amp;L83&amp;P83&amp;"
   outputResources = "&amp;T83&amp;X83&amp;AB83&amp;AF83&amp;"
@@ -13513,13 +13879,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C83" t="str">
+      <c r="C83" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E83),"",IF(Outputs!A83="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A83="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A83="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A83="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A83="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A83="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E83&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E83&amp;"
+  StartActionName = Start "&amp;$E83&amp;"
+  StopActionName = Stop "&amp;$E83&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G83&amp;I83&amp;M83&amp;Q83&amp;"
   outputResources = "&amp;U83&amp;Y83&amp;AC83&amp;AG83&amp;"
@@ -13597,7 +13965,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:33">
+    <row r="84" spans="1:33" ht="409">
       <c r="A84" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -13607,8 +13975,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E84&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E84&amp;"
+  StartActionName = Start "&amp;$E84&amp;"
+  StopActionName = Stop "&amp;$E84&amp;"
   conversionRate = 1
   inputResources = "&amp;$G84&amp;H84&amp;L84&amp;P84&amp;"
   outputResources = "&amp;T84&amp;X84&amp;AB84&amp;AF84&amp;"
@@ -13617,13 +13987,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C84" t="str">
+      <c r="C84" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E84),"",IF(Outputs!A84="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A84="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A84="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A84="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A84="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A84="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E84&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E84&amp;"
+  StartActionName = Start "&amp;$E84&amp;"
+  StopActionName = Stop "&amp;$E84&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G84&amp;I84&amp;M84&amp;Q84&amp;"
   outputResources = "&amp;U84&amp;Y84&amp;AC84&amp;AG84&amp;"
@@ -13701,7 +14073,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:33">
+    <row r="85" spans="1:33" ht="409">
       <c r="A85" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -13711,8 +14083,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E85&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E85&amp;"
+  StartActionName = Start "&amp;$E85&amp;"
+  StopActionName = Stop "&amp;$E85&amp;"
   conversionRate = 1
   inputResources = "&amp;$G85&amp;H85&amp;L85&amp;P85&amp;"
   outputResources = "&amp;T85&amp;X85&amp;AB85&amp;AF85&amp;"
@@ -13721,13 +14095,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C85" t="str">
+      <c r="C85" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E85),"",IF(Outputs!A85="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A85="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A85="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A85="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A85="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A85="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E85&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E85&amp;"
+  StartActionName = Start "&amp;$E85&amp;"
+  StopActionName = Stop "&amp;$E85&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G85&amp;I85&amp;M85&amp;Q85&amp;"
   outputResources = "&amp;U85&amp;Y85&amp;AC85&amp;AG85&amp;"
@@ -13805,7 +14181,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:33">
+    <row r="86" spans="1:33" ht="409">
       <c r="A86" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -13815,8 +14191,10 @@
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E86&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E86&amp;"
+  StartActionName = Start "&amp;$E86&amp;"
+  StopActionName = Stop "&amp;$E86&amp;"
   conversionRate = 1
   inputResources = "&amp;$G86&amp;H86&amp;L86&amp;P86&amp;"
   outputResources = "&amp;T86&amp;X86&amp;AB86&amp;AF86&amp;"
@@ -13825,13 +14203,15 @@
 ")</f>
         <v/>
       </c>
-      <c r="C86" t="str">
+      <c r="C86" s="6" t="str">
         <f>IF(ISBLANK(Outputs!E86),"",IF(Outputs!A86="Distiller","@PART[KA_Distiller_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A86="DistillerM","@PART[KA_Distiller_125_01M]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A86="ConverterC","@PART[KA_Converter_125_01]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A86="ConverterN","@PART[KA_Converter_125_01N]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A86="ConverterH","@PART[KA_Converter_125_01H]:AFTER[Karbonite]:NEEDS[RealFuels]",IF(Outputs!A86="ConverterO","@PART[KA_Converter_125_01O]:AFTER[Karbonite]:NEEDS[RealFuels]","ERROR!"))))))&amp;"
 {
  MODULE
  {
-  name = USI_Converter
-  converterName = "&amp;$E86&amp;"
+  name = REGO_ModuleResourceConverter
+  ConverterName = "&amp;$E86&amp;"
+  StartActionName = Start "&amp;$E86&amp;"
+  StopActionName = Stop "&amp;$E86&amp;"
   conversionRate = 0.5
   inputResources = "&amp;$G86&amp;I86&amp;M86&amp;Q86&amp;"
   outputResources = "&amp;U86&amp;Y86&amp;AC86&amp;AG86&amp;"
@@ -13910,11 +14290,11 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -13922,7 +14302,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFFFFFFF"/>
   </sheetPr>
@@ -13932,7 +14312,7 @@
       <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
@@ -14093,7 +14473,7 @@
       </c>
       <c r="H4">
         <f>E4/G4</f>
-        <v>1.0000000000000004</v>
+        <v>1.0000000000000007</v>
       </c>
       <c r="I4">
         <f>E4/C4</f>
@@ -14105,7 +14485,7 @@
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>2.0000000000000004</v>
+        <v>2.0000000000000009</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
@@ -14948,7 +15328,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <conditionalFormatting sqref="G16:J37">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>G16&gt;0</formula>
@@ -14956,7 +15335,7 @@
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>